<commit_message>
chore: up fix excel
</commit_message>
<xml_diff>
--- a/ui/public/modele-import.xlsx
+++ b/ui/public/modele-import.xlsx
@@ -1,22 +1,1718 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10719"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raph/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DB2679-BCDF-774B-9A60-C8B8EEDD5558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Modèle" sheetId="1" r:id="rId1"/>
+    <sheet name="Description des données" sheetId="2" r:id="rId2"/>
+  </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
+</workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="227">
+  <si>
+    <t>statut_apprenant</t>
+  </si>
+  <si>
+    <t>date_metier_mise_a_jour_statut</t>
+  </si>
+  <si>
+    <t>ine_apprenant</t>
+  </si>
+  <si>
+    <t>email_contact</t>
+  </si>
+  <si>
+    <t>tel_apprenant</t>
+  </si>
+  <si>
+    <t>libelle_court_formation</t>
+  </si>
+  <si>
+    <t>annee_formation</t>
+  </si>
+  <si>
+    <t>formation_rncp</t>
+  </si>
+  <si>
+    <t>contrat_date_debut</t>
+  </si>
+  <si>
+    <t>contrat_date_fin</t>
+  </si>
+  <si>
+    <t>contrat_date_rupture</t>
+  </si>
+  <si>
+    <t>nir_apprenant</t>
+  </si>
+  <si>
+    <t>adresse_apprenant</t>
+  </si>
+  <si>
+    <t>code_postal_apprenant</t>
+  </si>
+  <si>
+    <t>sexe_apprenant</t>
+  </si>
+  <si>
+    <t>rqth_apprenant</t>
+  </si>
+  <si>
+    <t>date_rqth_apprenant</t>
+  </si>
+  <si>
+    <t>responsable_apprenant_mail1</t>
+  </si>
+  <si>
+    <t>responsable_apprenant_mail2</t>
+  </si>
+  <si>
+    <t>obtention_diplome_formation</t>
+  </si>
+  <si>
+    <t>date_obtention_diplome_formation</t>
+  </si>
+  <si>
+    <t>date_exclusion_formation</t>
+  </si>
+  <si>
+    <t>cause_exclusion_formation</t>
+  </si>
+  <si>
+    <t>nom_referent_handicap_formation</t>
+  </si>
+  <si>
+    <t>prenom_referent_handicap_formation</t>
+  </si>
+  <si>
+    <t>email_referent_handicap_formation</t>
+  </si>
+  <si>
+    <t>cause_rupture_contrat</t>
+  </si>
+  <si>
+    <t>contrat_date_debut_2</t>
+  </si>
+  <si>
+    <t>contrat_date_fin_2</t>
+  </si>
+  <si>
+    <t>contrat_date_rupture_2</t>
+  </si>
+  <si>
+    <t>cause_rupture_contrat_2</t>
+  </si>
+  <si>
+    <t>contrat_date_debut_3</t>
+  </si>
+  <si>
+    <t>contrat_date_fin_3</t>
+  </si>
+  <si>
+    <t>contrat_date_rupture_3</t>
+  </si>
+  <si>
+    <t>cause_rupture_contrat_3</t>
+  </si>
+  <si>
+    <t>contrat_date_debut_4</t>
+  </si>
+  <si>
+    <t>contrat_date_fin_4</t>
+  </si>
+  <si>
+    <t>contrat_date_rupture_4</t>
+  </si>
+  <si>
+    <t>cause_rupture_contrat_4</t>
+  </si>
+  <si>
+    <t>siret_employeur</t>
+  </si>
+  <si>
+    <t>siret_employeur_2</t>
+  </si>
+  <si>
+    <t>siret_employeur_3</t>
+  </si>
+  <si>
+    <t>siret_employeur_4</t>
+  </si>
+  <si>
+    <t>formation_presentielle</t>
+  </si>
+  <si>
+    <t>Gaston</t>
+  </si>
+  <si>
+    <t>gaston.lenotre@domain.tld</t>
+  </si>
+  <si>
+    <t>CAP PATISSIER</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>escoffier@domain.tld</t>
+  </si>
+  <si>
+    <t>0123456A</t>
+  </si>
+  <si>
+    <t>50022141</t>
+  </si>
+  <si>
+    <t>2022-2023</t>
+  </si>
+  <si>
+    <t>nom_apprenant *</t>
+  </si>
+  <si>
+    <t>prenom_apprenant *</t>
+  </si>
+  <si>
+    <t>Nom du champ</t>
+  </si>
+  <si>
+    <t>Obligatoire</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Exemple</t>
+  </si>
+  <si>
+    <t>Pourquoi demande t-on cette donnée ?</t>
+  </si>
+  <si>
+    <t>(SIFA)</t>
+  </si>
+  <si>
+    <t>Informations concernant l'apprenant</t>
+  </si>
+  <si>
+    <t>Oui</t>
+  </si>
+  <si>
+    <t>nom de famille de l'apprenant</t>
+  </si>
+  <si>
+    <t>Alpha : au moins 1 lettre, espace/tiret/accent possibles - pas de chiffre. Caractères spéciaux acceptés</t>
+  </si>
+  <si>
+    <t>Dupuis</t>
+  </si>
+  <si>
+    <t>La clef d’unicité permettant d’identifier un apprenant unique et d’effectuer des opérations de dédoublonnage se compose de : Nom, Prénom, date de naissance, CFD de la formation, UAI de l’organisme de formation.</t>
+  </si>
+  <si>
+    <t>prénom de l'apprenant (uniquement le premier prénom)</t>
+  </si>
+  <si>
+    <t>date_de_naissance_apprenant *</t>
+  </si>
+  <si>
+    <t>date de naissance de l'apprenant</t>
+  </si>
+  <si>
+    <t>date à laquelle le statut de l'apprenant a été saisi</t>
+  </si>
+  <si>
+    <t>statut de l'apprenant (apprenti, inscrit sans contrat, abandon, rupturant)</t>
+  </si>
+  <si>
+    <t>Valeurs possibles : 0, 2, 3</t>
+  </si>
+  <si>
+    <t>Non</t>
+  </si>
+  <si>
+    <t>les coordonnées de contact sont notamment utilisées par les cellules d'accompagnement des décrocheurs</t>
+  </si>
+  <si>
+    <t>Numéro de téléphone portable ou fixe de l’apprenant</t>
+  </si>
+  <si>
+    <t>Identifiant National Élève, inscrit dans le "répertoire national des identifiants élèves, étudiants et apprentis</t>
+  </si>
+  <si>
+    <t>10 chiffres + 1 lettre, &gt; ou 9 chiffres + 2 lettres, &gt; ou 9 caractères alphanumériques + 1 chiffre.</t>
+  </si>
+  <si>
+    <t>Le NIR est aussi appelé "numéro de sécurité sociale". 
+2 chiffres constituant une « clé de contrôle » complètent le numéro de sécurité sociale. Cette clé de contrôle permet de vérifier que le numéro de sécurité sociale est bien formé.</t>
+  </si>
+  <si>
+    <t>13 chiffres</t>
+  </si>
+  <si>
+    <t>id_erp_apprenant *</t>
+  </si>
+  <si>
+    <t>clé d'identification unique de l'apprenant dans l'erp</t>
+  </si>
+  <si>
+    <t>chaine de caractères libre (générée par le système de gestion des apprenants)</t>
+  </si>
+  <si>
+    <t>A881F3</t>
+  </si>
+  <si>
+    <t>apprenant_rqth</t>
+  </si>
+  <si>
+    <t>date_reconnaissance_RQTH</t>
+  </si>
+  <si>
+    <t>date de reconnaissance du statut de travailleur handicapé de l'apprenant</t>
+  </si>
+  <si>
+    <t>apprenant_adresse</t>
+  </si>
+  <si>
+    <t>Adresse principale actuelle de l’apprenant.
+Indiquer :
+- le N° de la voie
+- (éventuellement l’indice de répétition)
+- la nature de la voie (Route, avenue, rue, Impasse, etc…)
+- le complément (Résidence, Immeuble, étage, porte)
+- le libellé de la voie</t>
+  </si>
+  <si>
+    <t>Chaîne de caractères alphanumériques</t>
+  </si>
+  <si>
+    <t>64 bis, route de Paris</t>
+  </si>
+  <si>
+    <t>Code postal du lieu d’habitation de l’apprenant</t>
+  </si>
+  <si>
+    <t>Suite numérique de 5 chiffres</t>
+  </si>
+  <si>
+    <t>apprenant_responsable_mail_1</t>
+  </si>
+  <si>
+    <t>courriel du 1er responsable légal de l'apprenant (parent ou tuteur)</t>
+  </si>
+  <si>
+    <t>Alpha numérique avec un @ : texte@texte.texte</t>
+  </si>
+  <si>
+    <t>apprenant_responsable_mail_2</t>
+  </si>
+  <si>
+    <t>courriel du 2eme responsable légal de l'apprenant (parent ou tuteur)</t>
+  </si>
+  <si>
+    <t>apprenant_sexe</t>
+  </si>
+  <si>
+    <t>Différentes valeurs acceptées : 1, 2 ou H, F ou M, F</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>statistiques répartition hommes/femmes</t>
+  </si>
+  <si>
+    <t>Informations concernant l'organisme de formation</t>
+  </si>
+  <si>
+    <t>etablissement_responsable_uai *</t>
+  </si>
+  <si>
+    <t>Unité Administrative Immatriculée de l'établissement signataire de la convention. La donnée “UAI” affichée provient de la base de données RAMSESE et notamment exploité par la DEC avant d’être validée au niveau de chaque territoire.</t>
+  </si>
+  <si>
+    <t>7 chiffres suivis d’une lettre, les trois premiers chiffres indiquant le département. 1234567A</t>
+  </si>
+  <si>
+    <t>etablissement_responsable_siret *</t>
+  </si>
+  <si>
+    <t>Système d'identification du répertoire des établissements. Code chiffré unique et officiel. Chaque établissement d’entreprise possède un SIRET. Il est attribué par l’INSEE, l’Institut National de la Statistique et des Etudes.</t>
+  </si>
+  <si>
+    <t>14 chiffres : les 9 chiffres du Siren + 5 chiffres propres à chaque établissement</t>
+  </si>
+  <si>
+    <t>etablissement_formateur_uai *</t>
+  </si>
+  <si>
+    <t>etablissement_formateur_siret *</t>
+  </si>
+  <si>
+    <t>etablissement_lieu_de_formation_uai *</t>
+  </si>
+  <si>
+    <t>C'est celui-ci qui sera utilisé partout pour identifier où est l'apprenant (organisme_id)</t>
+  </si>
+  <si>
+    <t>etablissement_lieu_de_formation_siret *</t>
+  </si>
+  <si>
+    <t>C'est celui-ci qui sera utilisé partout pour identifier où est l'apprenant</t>
+  </si>
+  <si>
+    <t>Informations concernant la formation suivie</t>
+  </si>
+  <si>
+    <t>année scolaire en cours pour l'apprenant.</t>
+  </si>
+  <si>
+    <t>AAAA-AAAA</t>
+  </si>
+  <si>
+    <t>année de formation concernée</t>
+  </si>
+  <si>
+    <t>Énumération : 1, 2, 3, 4, 5</t>
+  </si>
+  <si>
+    <t>Si c'est la deuxième année du CAP =&gt;2</t>
+  </si>
+  <si>
+    <t>date_inscription_formation *</t>
+  </si>
+  <si>
+    <t>Date à laquelle le jeune s’est inscrit sur sa formation (avec ou sans contrat)</t>
+  </si>
+  <si>
+    <t>date_entrée_formation *</t>
+  </si>
+  <si>
+    <t>Date à laquelle le jeune a démarré sa formation (avec ou sans contrat)</t>
+  </si>
+  <si>
+    <t>date_fin_formation *</t>
+  </si>
+  <si>
+    <t>date de fin prévisionnelle de la formation</t>
+  </si>
+  <si>
+    <t>formation_duree_theorique *</t>
+  </si>
+  <si>
+    <t>durée théorique de la formation</t>
+  </si>
+  <si>
+    <t>minimum : 1 / minimum 4</t>
+  </si>
+  <si>
+    <t>Libellé court de la formation</t>
+  </si>
+  <si>
+    <t>Suite de caractères alphanumériques</t>
+  </si>
+  <si>
+    <t>Oui, facultatif si RNCP collectable</t>
+  </si>
+  <si>
+    <t>Permet, par l’usage de ce code, d’identifier la formation concernée et les effectifs par typologie de formations et par secteur.</t>
+  </si>
+  <si>
+    <t>5729454F</t>
+  </si>
+  <si>
+    <t>Oui, facultatif si cfd collectable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code RNCP (Répertoire National des Certifications Professionnelles) de la formation suivie. Permet, par l’usage de ce code, d'identifier la formation concernée et pouvoir identifier les effectifs par typologie de formations et par secteur.
+</t>
+  </si>
+  <si>
+    <t>date_declaration_1ere_absence_formation</t>
+  </si>
+  <si>
+    <t>permet de détecter un risque d'abandon</t>
+  </si>
+  <si>
+    <t>date_declaration_2e_absence_formation</t>
+  </si>
+  <si>
+    <t>permet de détecter un risque de décrochage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cause_exclusion_formation
+</t>
+  </si>
+  <si>
+    <t>Suite de caractères alphanumériques (champ libre)</t>
+  </si>
+  <si>
+    <t>absences répétées et injustifiées</t>
+  </si>
+  <si>
+    <t>permet de proposer un service d'accompagnement adapté pour éviter un risque de décrochage)</t>
+  </si>
+  <si>
+    <t>obtention_diplome _annee N</t>
+  </si>
+  <si>
+    <t>le diplôme a été ou non obtenu à l'issue de la formation</t>
+  </si>
+  <si>
+    <t>date_obtention_diplome_annee N</t>
+  </si>
+  <si>
+    <t>date d'obtention du diplôme correspondant à la formation. À remplir si le diplôme a été obtenu</t>
+  </si>
+  <si>
+    <t>s'il y en a un affecté à cette formation</t>
+  </si>
+  <si>
+    <t>Séries de lettres</t>
+  </si>
+  <si>
+    <t>Dumas</t>
+  </si>
+  <si>
+    <t>permet de communiquer l'information aux services d'accompagnement</t>
+  </si>
+  <si>
+    <t>Sylvie</t>
+  </si>
+  <si>
+    <t>mail_referent_handicap_formation</t>
+  </si>
+  <si>
+    <t>Alpha numérique avec un @ et un “.” : texte@texte.texte</t>
+  </si>
+  <si>
+    <t>Formation_presentielle</t>
+  </si>
+  <si>
+    <t>formation 100% à distance ou non (mettre non si 100% à distance ?)</t>
+  </si>
+  <si>
+    <t>Informations concernant l'employeur et le contrat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">employeur_siret 
+</t>
+  </si>
+  <si>
+    <t>siret de l'employeur chez qui est réalisé le 1er contrat d'apprentissage</t>
+  </si>
+  <si>
+    <t>Numérique sur 14 positions sans espaces : les 9 chiffres du numéro SIREN + les 5 chiffres du NIC - espace possible - suppression des espaces à l'enregistrement</t>
+  </si>
+  <si>
+    <t>Date de début du 1er contrat initial en apprentissage.
+Se référer à la date du CERFA ou de la Convention</t>
+  </si>
+  <si>
+    <t>Date de fin du 1er contrat initial en apprentissage.
+Se référer à la date du CERFA ou de la Convention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contrat_date_rupture
+</t>
+  </si>
+  <si>
+    <t>Oui, s'il y a rupture dans le contrat d'apprentissage</t>
+  </si>
+  <si>
+    <t>Date de rupture du 1er contrat initial en apprentissage.
+Se référer à la date du CERFA ou de la Convention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contrat_cause_rupture
+</t>
+  </si>
+  <si>
+    <t>nomenclature à fournir ou envoi champ texte libre</t>
+  </si>
+  <si>
+    <t>Faute lourde</t>
+  </si>
+  <si>
+    <t>siret de l'employeur chez qui est réalisé le 2e contrat après rupture du 1er contrat</t>
+  </si>
+  <si>
+    <t>contrat_2_date_debut</t>
+  </si>
+  <si>
+    <t>Date de début du 2eme contrat initial en apprentissage suite à la rupture du 1er contrat.
+Se référer à la date du CERFA ou de la Convention</t>
+  </si>
+  <si>
+    <t>contrat_2_date_fin</t>
+  </si>
+  <si>
+    <t>Date de fin du 2eme contrat initial en apprentissage suite à la rupture du 1er contrat.
+Se référer à la date du CERFA ou de la Convention</t>
+  </si>
+  <si>
+    <t>contrat_2_date_rupture
+récupérer donnée auprès de datalake pole emploi ? (cf attestation de fin de contrat télétransmise par les employeurs à pole emploi)</t>
+  </si>
+  <si>
+    <t>Date de rupture du 2eme contrat initial en apprentissage.
+Se référer à la date du CERFA ou de la Convention</t>
+  </si>
+  <si>
+    <t>contrat_2_cause_rupture
+récupérer donnée auprès de datalake pole emploi ? (cf attestation de fin de contrat télétransmise par les employeurs à pole emploi)</t>
+  </si>
+  <si>
+    <t>cause de la rupture du 2eme contrat d'apprentissage</t>
+  </si>
+  <si>
+    <t>siret de l'employeur chez qui est réalisé le 3e contrat après rupture du 2e contrat</t>
+  </si>
+  <si>
+    <t>contrat_3_date_debut</t>
+  </si>
+  <si>
+    <t>Date de début du 3eme contrat initial en apprentissage après rupture du 2eme contrat.
+Se référer à la date du CERFA ou de la Convention</t>
+  </si>
+  <si>
+    <t>contrat_3_date_fin</t>
+  </si>
+  <si>
+    <t>date de fin prévisionnelle du 3e contrat d'apprentissage</t>
+  </si>
+  <si>
+    <t>contrat_3_date_rupture</t>
+  </si>
+  <si>
+    <t>date de rupture du 3e contrat</t>
+  </si>
+  <si>
+    <t>contrat_3_cause_rupture</t>
+  </si>
+  <si>
+    <t>cause de la rupture du 3e contrat d'apprentissage (nomenclature à fournir ou envoi champ texte libre)</t>
+  </si>
+  <si>
+    <t>Obtention du diplôme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">courriel de l'apprenant </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alpha numérique avec un @ et un “.”  texte@texte.texte
+</t>
+  </si>
+  <si>
+    <t>Suite numérique au choix : 
+- 10 caractères numériques commençant par 1 zéro - espace/tiret/point possible à la saisie, retrait lors du traitement
+-  Indicateur national (+33) + 9 caractères numériques</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nir_apprenant </t>
+  </si>
+  <si>
+    <t xml:space="preserve">statut de travailleur handicapé de l'apprenant </t>
+  </si>
+  <si>
+    <t xml:space="preserve">apprenant_code_postal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genre, sexe de l'apprenant </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UAI du lieu de formation. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">annee_scolaire  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNCP + 5 chiffres (RNCPXXXXX) ou 5 chiffre. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">date de la 1ère absence en formation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mis par raph comme étant hors du périmètre finalement est-ce que c'est vraiment le cas ? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">date de la 2ème absence en formation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">date d'exclusion de la formation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cause d'exclusion de la formation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">s'il y en a un affecté à cette formation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cause de la rupture du 1er contrat d'apprentissage </t>
+  </si>
+  <si>
+    <t>06 12 34 56 78</t>
+  </si>
+  <si>
+    <t>absences répétées</t>
+  </si>
+  <si>
+    <t>formation_cfd *</t>
+  </si>
+  <si>
+    <t>date_entree_formation *</t>
+  </si>
+  <si>
+    <t>duree_theorique_formation *</t>
+  </si>
+  <si>
+    <t>annee_scolaire *</t>
+  </si>
+  <si>
+    <t>statut_apprenant *</t>
+  </si>
+  <si>
+    <t>date_metier_mise_a_jour_statut *</t>
+  </si>
+  <si>
+    <t>1234567890A</t>
+  </si>
+  <si>
+    <t>(Norme ISO-8601). AAAA-MM-JJ ou JJ/MM/AAAA</t>
+  </si>
+  <si>
+    <t>0 = abandon
+2 = inscrit
+3 = apprenti</t>
+  </si>
+  <si>
+    <t>0612345678 ou (+)33612345678</t>
+  </si>
+  <si>
+    <t>Permet d'avoir un identifiant unique pour l'apprenant</t>
+  </si>
+  <si>
+    <t>booléen : VRAI / FAUX</t>
+  </si>
+  <si>
+    <t>marc.dupuis@domain.tld</t>
+  </si>
+  <si>
+    <t>jeanne.dupuis@domain.tld</t>
+  </si>
+  <si>
+    <t>formation_cfd*</t>
+  </si>
+  <si>
+    <t>formation_rncp  *</t>
+  </si>
+  <si>
+    <t>RNCP12345</t>
+  </si>
+  <si>
+    <t>Booléen (VRAI / FAUX)</t>
+  </si>
+  <si>
+    <t>Lenôtre</t>
+  </si>
+</sst>
+</file>
+
+<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+  </fonts>
+  <fills count="4">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFDD02"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFE2F3"/>
+        <bgColor rgb="FFCFE2F3"/>
+      </patternFill>
+    </fill>
+  </fills>
+  <borders count="5">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="31">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+  </cellXfs>
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF666666"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666666"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFDD02"/>
+      <color rgb="FFFFD579"/>
+    </mruColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
+</styleSheet>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+  <a:themeElements>
+    <a:clrScheme name="Office 2007 - 2010">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office 2007 - 2010">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office 2007 - 2010">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BH2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="26.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="26.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="31" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="30.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="33.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="31.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="35" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="39" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="43" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="48" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="23.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="24.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="28.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="26" style="1" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="27.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="33.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="34.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="61" max="16384" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:60" s="9" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="AN1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AQ1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AR1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AS1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AT1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="AU1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AV1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AW1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="AX1" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="AY1" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="AZ1" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="BA1" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="BB1" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="BC1" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="BD1" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="BE1" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="BF1" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="BG1" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="BH1" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:60" s="10" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="11">
+        <v>36827</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="10">
+        <v>0</v>
+      </c>
+      <c r="F2" s="11">
+        <v>36827</v>
+      </c>
+      <c r="G2" s="10">
+        <v>1111111</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" s="10">
+        <v>1</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="N2" s="11">
+        <v>44937</v>
+      </c>
+      <c r="O2" s="11">
+        <v>45087</v>
+      </c>
+      <c r="P2" s="11">
+        <v>45087</v>
+      </c>
+      <c r="Q2" s="10" t="str">
+        <f>"1234567890123"</f>
+        <v>1234567890123</v>
+      </c>
+      <c r="R2" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="S2" s="10">
+        <v>44000</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="U2" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="V2" s="11">
+        <v>40479</v>
+      </c>
+      <c r="W2" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="X2" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y2" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="11">
+        <v>45087</v>
+      </c>
+      <c r="AA2" s="11">
+        <v>45087</v>
+      </c>
+      <c r="AF2" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="AG2" s="11">
+        <v>44937</v>
+      </c>
+      <c r="AH2" s="11">
+        <v>45087</v>
+      </c>
+      <c r="AI2" s="11">
+        <v>45087</v>
+      </c>
+      <c r="AS2" s="10" t="str">
+        <f>"12345678901235"</f>
+        <v>12345678901235</v>
+      </c>
+      <c r="AT2" s="10" t="str">
+        <f>"12345678901235"</f>
+        <v>12345678901235</v>
+      </c>
+      <c r="AU2" s="10" t="str">
+        <f>"12345678901237"</f>
+        <v>12345678901237</v>
+      </c>
+      <c r="AV2" s="10" t="str">
+        <f>"12345678901238"</f>
+        <v>12345678901238</v>
+      </c>
+      <c r="AW2" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX2" s="11">
+        <v>44937</v>
+      </c>
+      <c r="AY2" s="11">
+        <v>44937</v>
+      </c>
+      <c r="AZ2" s="11">
+        <v>45087</v>
+      </c>
+      <c r="BA2" s="10">
+        <v>4</v>
+      </c>
+      <c r="BB2" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="BC2" s="10" t="str">
+        <f>"12345678901235"</f>
+        <v>12345678901235</v>
+      </c>
+      <c r="BD2" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="BE2" s="10" t="str">
+        <f>"12345678901235"</f>
+        <v>12345678901235</v>
+      </c>
+      <c r="BF2" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="BG2" s="10" t="str">
+        <f>"12345678901235"</f>
+        <v>12345678901235</v>
+      </c>
+      <c r="BH2" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587136C3-4E68-704D-AFDE-CEF947822B6E}">
   <dimension ref="A1:AA978"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="35.1640625" style="22" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" style="22" customWidth="1"/>
-    <col min="4" max="4" width="48.83203125" style="22" customWidth="1"/>
-    <col min="5" max="5" width="24" style="22" customWidth="1"/>
-    <col min="6" max="6" width="23.5" style="22" customWidth="1"/>
-    <col min="7" max="7" width="34.33203125" style="22" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" style="22" customWidth="1"/>
-    <col min="9" max="16384" width="12.6640625" style="22"/>
+    <col min="1" max="2" width="35.1640625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="48.83203125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="24" style="16" customWidth="1"/>
+    <col min="6" max="6" width="23.5" style="16" customWidth="1"/>
+    <col min="7" max="7" width="34.33203125" style="16" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" style="16" customWidth="1"/>
+    <col min="9" max="16384" width="12.6640625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15" x14ac:dyDescent="0.2">
@@ -63,7 +1759,7 @@
       <c r="AA1" s="2"/>
     </row>
     <row r="2" spans="1:27" ht="60" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>61</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -81,12 +1777,12 @@
       <c r="F2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="12" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="60" x14ac:dyDescent="0.2">
-      <c r="A3" s="23"/>
+      <c r="A3" s="17"/>
       <c r="B3" s="4" t="s">
         <v>53</v>
       </c>
@@ -100,12 +1796,12 @@
         <v>64</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="24"/>
+        <v>44</v>
+      </c>
+      <c r="G3" s="17"/>
     </row>
     <row r="4" spans="1:27" ht="30" x14ac:dyDescent="0.2">
-      <c r="A4" s="23"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="4" t="s">
         <v>68</v>
       </c>
@@ -115,17 +1811,17 @@
       <c r="D4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E4" s="17" t="s">
-        <v>219</v>
+      <c r="E4" s="4" t="s">
+        <v>215</v>
       </c>
       <c r="F4" s="5">
         <v>35819</v>
       </c>
-      <c r="G4" s="24"/>
+      <c r="G4" s="17"/>
     </row>
     <row r="5" spans="1:27" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="23"/>
-      <c r="B5" s="16" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -134,17 +1830,17 @@
       <c r="D5" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>219</v>
+      <c r="E5" s="4" t="s">
+        <v>215</v>
       </c>
       <c r="F5" s="5">
         <v>35819</v>
       </c>
-      <c r="G5" s="17"/>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:27" ht="45" x14ac:dyDescent="0.2">
-      <c r="A6" s="23"/>
-      <c r="B6" s="16" t="s">
+      <c r="A6" s="17"/>
+      <c r="B6" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -153,18 +1849,18 @@
       <c r="D6" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F6" s="4">
         <v>2</v>
       </c>
-      <c r="G6" s="17" t="s">
-        <v>217</v>
+      <c r="G6" s="4" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="45" x14ac:dyDescent="0.2">
-      <c r="A7" s="23"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
@@ -177,15 +1873,15 @@
       <c r="E7" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="F7" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" s="21" t="s">
+      <c r="F7" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="20" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="105" x14ac:dyDescent="0.2">
-      <c r="A8" s="23"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
@@ -198,205 +1894,205 @@
       <c r="E8" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="F8" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="G8" s="21" t="s">
+      <c r="F8" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="G8" s="20" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="60" x14ac:dyDescent="0.2">
-      <c r="A9" s="23"/>
-      <c r="B9" s="17" t="s">
+      <c r="A9" s="17"/>
+      <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="G9" s="17" t="s">
-        <v>215</v>
+      <c r="G9" s="4" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="60" x14ac:dyDescent="0.2">
-      <c r="A10" s="23"/>
-      <c r="B10" s="17" t="s">
+      <c r="A10" s="17"/>
+      <c r="B10" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F10" s="17" t="str">
+      <c r="F10" s="4" t="str">
         <f>"1234567890123"</f>
         <v>1234567890123</v>
       </c>
-      <c r="G10" s="17"/>
+      <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:27" ht="45" x14ac:dyDescent="0.2">
-      <c r="A11" s="23"/>
-      <c r="B11" s="17" t="s">
+      <c r="A11" s="17"/>
+      <c r="B11" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G11" s="17"/>
+      <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="23"/>
-      <c r="B12" s="17" t="s">
+      <c r="A12" s="17"/>
+      <c r="B12" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="E12" s="17" t="s">
-        <v>218</v>
-      </c>
-      <c r="F12" s="17" t="b">
+      <c r="E12" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="F12" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="G12" s="17"/>
+      <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:27" ht="30" x14ac:dyDescent="0.2">
-      <c r="A13" s="23"/>
-      <c r="B13" s="17" t="s">
+      <c r="A13" s="17"/>
+      <c r="B13" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E13" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="F13" s="19">
+      <c r="E13" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F13" s="5">
         <v>45160</v>
       </c>
-      <c r="G13" s="17"/>
+      <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:27" ht="105" x14ac:dyDescent="0.2">
-      <c r="A14" s="23"/>
-      <c r="B14" s="17" t="s">
+      <c r="A14" s="17"/>
+      <c r="B14" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="G14" s="17"/>
+      <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="23"/>
-      <c r="B15" s="17" t="s">
+      <c r="A15" s="17"/>
+      <c r="B15" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="F15" s="21">
+      <c r="F15" s="20">
         <v>44000</v>
       </c>
-      <c r="G15" s="17"/>
+      <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:27" ht="30" x14ac:dyDescent="0.2">
-      <c r="A16" s="23"/>
-      <c r="B16" s="17" t="s">
+      <c r="A16" s="17"/>
+      <c r="B16" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F16" s="25" t="s">
+      <c r="F16" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="G16" s="17"/>
-    </row>
-    <row r="17" spans="1:27" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" s="23"/>
-      <c r="B17" s="17" t="s">
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:27" ht="30" x14ac:dyDescent="0.2">
+      <c r="A17" s="17"/>
+      <c r="B17" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="26" t="s">
+      <c r="F17" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="G17" s="17"/>
+      <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:27" ht="30" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="6" t="s">
         <v>98</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F18" s="28" t="s">
+      <c r="F18" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="G18" s="30" t="s">
+      <c r="G18" s="23" t="s">
         <v>101</v>
       </c>
       <c r="H18" s="7"/>
@@ -424,114 +2120,114 @@
       <c r="A19" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17" t="s">
+      <c r="C19" s="4"/>
+      <c r="D19" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="F19" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="G19" s="17"/>
+      <c r="F19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:27" ht="60" x14ac:dyDescent="0.2">
-      <c r="A20" s="23"/>
-      <c r="B20" s="17" t="s">
+      <c r="A20" s="17"/>
+      <c r="B20" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="17" t="s">
+      <c r="C20" s="20"/>
+      <c r="D20" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="4" t="s">
         <v>108</v>
       </c>
       <c r="F20" s="10" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
-      <c r="G20" s="17"/>
+      <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:27" ht="60" x14ac:dyDescent="0.2">
-      <c r="A21" s="23"/>
-      <c r="B21" s="17" t="s">
+      <c r="A21" s="17"/>
+      <c r="B21" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C21" s="21"/>
-      <c r="D21" s="17" t="s">
+      <c r="C21" s="20"/>
+      <c r="D21" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E21" s="21" t="s">
+      <c r="E21" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="F21" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="G21" s="17"/>
+      <c r="F21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:27" ht="60" x14ac:dyDescent="0.2">
-      <c r="A22" s="23"/>
-      <c r="B22" s="17" t="s">
+      <c r="A22" s="17"/>
+      <c r="B22" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="17" t="s">
+      <c r="C22" s="20"/>
+      <c r="D22" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="4" t="s">
         <v>108</v>
       </c>
       <c r="F22" s="10" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
-      <c r="G22" s="17"/>
+      <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:27" ht="45" x14ac:dyDescent="0.2">
-      <c r="A23" s="23"/>
-      <c r="B23" s="17" t="s">
+      <c r="A23" s="17"/>
+      <c r="B23" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="E23" s="21" t="s">
+      <c r="E23" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="F23" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="G23" s="21" t="s">
+      <c r="F23" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G23" s="20" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:27" ht="60" x14ac:dyDescent="0.2">
-      <c r="A24" s="12"/>
-      <c r="B24" s="28" t="s">
+      <c r="A24" s="13"/>
+      <c r="B24" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C24" s="28" t="s">
+      <c r="C24" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D24" s="28" t="s">
+      <c r="D24" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E24" s="28" t="s">
+      <c r="E24" s="6" t="s">
         <v>108</v>
       </c>
       <c r="F24" s="10" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
-      <c r="G24" s="30" t="s">
+      <c r="G24" s="23" t="s">
         <v>114</v>
       </c>
       <c r="H24" s="7"/>
@@ -556,390 +2252,390 @@
       <c r="AA24" s="7"/>
     </row>
     <row r="25" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="17" t="s">
+      <c r="D25" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="E25" s="17" t="s">
+      <c r="E25" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="F25" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G25" s="17"/>
+      <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:27" ht="30" x14ac:dyDescent="0.2">
-      <c r="A26" s="24"/>
-      <c r="B26" s="17" t="s">
+      <c r="A26" s="17"/>
+      <c r="B26" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="E26" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="F26" s="21" t="s">
+      <c r="F26" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="G26" s="17"/>
+      <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:27" ht="30" x14ac:dyDescent="0.2">
-      <c r="A27" s="24"/>
-      <c r="B27" s="17" t="s">
+      <c r="A27" s="17"/>
+      <c r="B27" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="D27" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E27" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="F27" s="32">
+      <c r="E27" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F27" s="24">
         <v>44832</v>
       </c>
-      <c r="G27" s="17"/>
+      <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:27" ht="30" x14ac:dyDescent="0.2">
-      <c r="A28" s="24"/>
-      <c r="B28" s="17" t="s">
+      <c r="A28" s="17"/>
+      <c r="B28" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D28" s="17" t="s">
+      <c r="D28" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="E28" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="F28" s="32">
+      <c r="E28" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F28" s="24">
         <v>44832</v>
       </c>
-      <c r="G28" s="17"/>
+      <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:27" ht="30" x14ac:dyDescent="0.2">
-      <c r="A29" s="24"/>
-      <c r="B29" s="17" t="s">
+      <c r="A29" s="17"/>
+      <c r="B29" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D29" s="17" t="s">
+      <c r="D29" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="E29" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="F29" s="32">
+      <c r="E29" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F29" s="24">
         <v>44832</v>
       </c>
-      <c r="G29" s="17"/>
+      <c r="G29" s="4"/>
     </row>
     <row r="30" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="24"/>
-      <c r="B30" s="17" t="s">
+      <c r="A30" s="17"/>
+      <c r="B30" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D30" s="17" t="s">
+      <c r="D30" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="E30" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="F30" s="17">
+      <c r="F30" s="4">
         <v>2</v>
       </c>
-      <c r="G30" s="17"/>
+      <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:27" ht="30" x14ac:dyDescent="0.2">
-      <c r="A31" s="24"/>
-      <c r="B31" s="17" t="s">
+      <c r="A31" s="17"/>
+      <c r="B31" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D31" s="17" t="s">
+      <c r="D31" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="F31" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="G31" s="17"/>
+      <c r="F31" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:27" ht="45" x14ac:dyDescent="0.2">
-      <c r="A32" s="24"/>
-      <c r="B32" s="17" t="s">
+      <c r="A32" s="17"/>
+      <c r="B32" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D32" s="17" t="s">
+      <c r="D32" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="E32" s="21" t="s">
+      <c r="E32" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="F32" s="17" t="s">
+      <c r="F32" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="G32" s="17"/>
+      <c r="G32" s="4"/>
     </row>
     <row r="33" spans="1:27" ht="75" x14ac:dyDescent="0.2">
-      <c r="A33" s="24"/>
-      <c r="B33" s="17" t="s">
+      <c r="A33" s="17"/>
+      <c r="B33" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C33" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="D33" s="17" t="s">
+      <c r="D33" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E33" s="17" t="s">
+      <c r="E33" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="F33" s="17" t="s">
+      <c r="F33" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="G33" s="17" t="s">
+      <c r="G33" s="4" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:27" ht="30" x14ac:dyDescent="0.2">
-      <c r="A34" s="24"/>
-      <c r="B34" s="17" t="s">
+      <c r="A34" s="17"/>
+      <c r="B34" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C34" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D34" s="17" t="s">
+      <c r="D34" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="E34" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="F34" s="32">
+      <c r="E34" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F34" s="24">
         <v>44832</v>
       </c>
-      <c r="G34" s="21" t="s">
+      <c r="G34" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="H34" s="14" t="s">
+      <c r="H34" s="12" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="35" spans="1:27" ht="30" x14ac:dyDescent="0.2">
-      <c r="A35" s="24"/>
-      <c r="B35" s="17" t="s">
+      <c r="A35" s="17"/>
+      <c r="B35" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D35" s="17" t="s">
+      <c r="D35" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="E35" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="F35" s="32">
+      <c r="E35" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F35" s="24">
         <v>44832</v>
       </c>
-      <c r="G35" s="21" t="s">
+      <c r="G35" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="H35" s="23"/>
+      <c r="H35" s="17"/>
     </row>
     <row r="36" spans="1:27" ht="30" x14ac:dyDescent="0.2">
-      <c r="A36" s="24"/>
-      <c r="B36" s="17" t="s">
+      <c r="A36" s="17"/>
+      <c r="B36" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C36" s="17" t="s">
+      <c r="C36" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D36" s="17" t="s">
+      <c r="D36" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="E36" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="F36" s="32">
+      <c r="E36" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F36" s="24">
         <v>44832</v>
       </c>
-      <c r="G36" s="17" t="s">
+      <c r="G36" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="H36" s="23"/>
+      <c r="H36" s="17"/>
     </row>
     <row r="37" spans="1:27" ht="45" x14ac:dyDescent="0.2">
-      <c r="A37" s="24"/>
-      <c r="B37" s="17" t="s">
+      <c r="A37" s="17"/>
+      <c r="B37" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C37" s="17" t="s">
+      <c r="C37" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D37" s="17" t="s">
+      <c r="D37" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="E37" s="17" t="s">
+      <c r="E37" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="F37" s="17" t="s">
+      <c r="F37" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="G37" s="17" t="s">
+      <c r="G37" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="H37" s="23"/>
+      <c r="H37" s="17"/>
     </row>
     <row r="38" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A38" s="24"/>
-      <c r="B38" s="17" t="s">
+      <c r="A38" s="17"/>
+      <c r="B38" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C38" s="17" t="s">
+      <c r="C38" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="17" t="s">
+      <c r="D38" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="E38" s="21" t="s">
+      <c r="E38" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="F38" s="17" t="b">
+      <c r="F38" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="G38" s="17"/>
+      <c r="G38" s="4"/>
     </row>
     <row r="39" spans="1:27" ht="30" x14ac:dyDescent="0.2">
-      <c r="A39" s="24"/>
-      <c r="B39" s="17" t="s">
+      <c r="A39" s="17"/>
+      <c r="B39" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="C39" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D39" s="17" t="s">
+      <c r="D39" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="E39" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="F39" s="32">
+      <c r="E39" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F39" s="24">
         <v>44832</v>
       </c>
-      <c r="G39" s="17"/>
+      <c r="G39" s="4"/>
     </row>
     <row r="40" spans="1:27" ht="30" x14ac:dyDescent="0.2">
-      <c r="A40" s="24"/>
-      <c r="B40" s="17" t="s">
+      <c r="A40" s="17"/>
+      <c r="B40" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C40" s="17" t="s">
+      <c r="C40" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D40" s="17" t="s">
+      <c r="D40" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="E40" s="17" t="s">
+      <c r="E40" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="F40" s="17" t="s">
+      <c r="F40" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="G40" s="21" t="s">
+      <c r="G40" s="20" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="41" spans="1:27" ht="30" x14ac:dyDescent="0.2">
-      <c r="A41" s="24"/>
-      <c r="B41" s="17" t="s">
+      <c r="A41" s="17"/>
+      <c r="B41" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C41" s="17" t="s">
+      <c r="C41" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D41" s="17" t="s">
+      <c r="D41" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="E41" s="17" t="s">
+      <c r="E41" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="F41" s="17" t="s">
+      <c r="F41" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="G41" s="21" t="s">
+      <c r="G41" s="20" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="42" spans="1:27" ht="30" x14ac:dyDescent="0.2">
-      <c r="A42" s="24"/>
-      <c r="B42" s="17" t="s">
+      <c r="A42" s="17"/>
+      <c r="B42" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C42" s="17" t="s">
+      <c r="C42" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D42" s="17" t="s">
+      <c r="D42" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="E42" s="17" t="s">
+      <c r="E42" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="F42" s="26" t="s">
+      <c r="F42" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="G42" s="21" t="s">
+      <c r="G42" s="20" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="43" spans="1:27" ht="30" x14ac:dyDescent="0.2">
-      <c r="A43" s="33"/>
-      <c r="B43" s="28" t="s">
+    <row r="43" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A43" s="13"/>
+      <c r="B43" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="C43" s="28" t="s">
+      <c r="C43" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D43" s="28" t="s">
+      <c r="D43" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="E43" s="35" t="s">
+      <c r="E43" s="25" t="s">
         <v>225</v>
       </c>
-      <c r="F43" s="34" t="b">
+      <c r="F43" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="G43" s="28"/>
-      <c r="H43" s="29"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="7"/>
       <c r="I43" s="7"/>
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
@@ -961,294 +2657,294 @@
       <c r="AA43" s="7"/>
     </row>
     <row r="44" spans="1:27" ht="75" x14ac:dyDescent="0.2">
-      <c r="A44" s="38" t="s">
+      <c r="A44" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="B44" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="C44" s="17" t="s">
+      <c r="C44" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D44" s="17" t="s">
+      <c r="D44" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="E44" s="17" t="s">
+      <c r="E44" s="4" t="s">
         <v>161</v>
       </c>
       <c r="F44" s="10" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
-      <c r="G44" s="17"/>
+      <c r="G44" s="4"/>
     </row>
     <row r="45" spans="1:27" ht="30" x14ac:dyDescent="0.2">
-      <c r="A45" s="39"/>
-      <c r="B45" s="17" t="s">
+      <c r="A45" s="17"/>
+      <c r="B45" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C45" s="17" t="s">
+      <c r="C45" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D45" s="17" t="s">
+      <c r="D45" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="E45" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="F45" s="32">
+      <c r="E45" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F45" s="24">
         <v>44937</v>
       </c>
-      <c r="G45" s="17"/>
+      <c r="G45" s="4"/>
     </row>
     <row r="46" spans="1:27" ht="30" x14ac:dyDescent="0.2">
-      <c r="A46" s="39"/>
-      <c r="B46" s="17" t="s">
+      <c r="A46" s="17"/>
+      <c r="B46" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C46" s="17" t="s">
+      <c r="C46" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D46" s="17" t="s">
+      <c r="D46" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="E46" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="F46" s="32">
+      <c r="E46" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F46" s="24">
         <v>45454</v>
       </c>
-      <c r="G46" s="17"/>
+      <c r="G46" s="4"/>
     </row>
     <row r="47" spans="1:27" ht="45" x14ac:dyDescent="0.2">
-      <c r="A47" s="39"/>
-      <c r="B47" s="17" t="s">
+      <c r="A47" s="17"/>
+      <c r="B47" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="C47" s="17" t="s">
+      <c r="C47" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D47" s="17" t="s">
+      <c r="D47" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E47" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="F47" s="32">
+      <c r="E47" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F47" s="24">
         <v>45454</v>
       </c>
-      <c r="G47" s="17"/>
+      <c r="G47" s="4"/>
     </row>
     <row r="48" spans="1:27" ht="45" x14ac:dyDescent="0.2">
-      <c r="A48" s="39"/>
-      <c r="B48" s="17" t="s">
+      <c r="A48" s="17"/>
+      <c r="B48" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D48" s="17" t="s">
+      <c r="D48" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="E48" s="21" t="s">
+      <c r="E48" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="F48" s="17" t="s">
+      <c r="F48" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="G48" s="17"/>
+      <c r="G48" s="4"/>
     </row>
     <row r="49" spans="1:7" ht="75" x14ac:dyDescent="0.2">
-      <c r="A49" s="39"/>
-      <c r="B49" s="17" t="s">
+      <c r="A49" s="17"/>
+      <c r="B49" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C49" s="17" t="s">
+      <c r="C49" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D49" s="17" t="s">
+      <c r="D49" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="E49" s="17" t="s">
+      <c r="E49" s="4" t="s">
         <v>161</v>
       </c>
       <c r="F49" s="10" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
-      <c r="G49" s="17"/>
+      <c r="G49" s="4"/>
     </row>
     <row r="50" spans="1:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="A50" s="39"/>
-      <c r="B50" s="17" t="s">
+      <c r="A50" s="17"/>
+      <c r="B50" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="C50" s="17" t="s">
+      <c r="C50" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D50" s="17" t="s">
+      <c r="D50" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="E50" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="F50" s="32">
+      <c r="E50" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F50" s="24">
         <v>44937</v>
       </c>
-      <c r="G50" s="17"/>
+      <c r="G50" s="4"/>
     </row>
     <row r="51" spans="1:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="A51" s="39"/>
-      <c r="B51" s="17" t="s">
+      <c r="A51" s="17"/>
+      <c r="B51" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="C51" s="17" t="s">
+      <c r="C51" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D51" s="17" t="s">
+      <c r="D51" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="E51" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="F51" s="32">
+      <c r="E51" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F51" s="24">
         <v>45454</v>
       </c>
-      <c r="G51" s="17"/>
+      <c r="G51" s="4"/>
     </row>
     <row r="52" spans="1:7" ht="60" x14ac:dyDescent="0.2">
-      <c r="A52" s="39"/>
-      <c r="B52" s="36" t="s">
+      <c r="A52" s="17"/>
+      <c r="B52" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="C52" s="17" t="s">
+      <c r="C52" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D52" s="17" t="s">
+      <c r="D52" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E52" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="F52" s="32">
+      <c r="E52" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F52" s="24">
         <v>45454</v>
       </c>
-      <c r="G52" s="17"/>
+      <c r="G52" s="4"/>
     </row>
     <row r="53" spans="1:7" ht="60" x14ac:dyDescent="0.2">
-      <c r="A53" s="39"/>
-      <c r="B53" s="36" t="s">
+      <c r="A53" s="17"/>
+      <c r="B53" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="C53" s="17" t="s">
+      <c r="C53" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D53" s="17" t="s">
+      <c r="D53" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="E53" s="21" t="s">
+      <c r="E53" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="F53" s="32">
+      <c r="F53" s="24">
         <v>45454</v>
       </c>
-      <c r="G53" s="17"/>
+      <c r="G53" s="4"/>
     </row>
     <row r="54" spans="1:7" ht="75" x14ac:dyDescent="0.2">
-      <c r="A54" s="39"/>
-      <c r="B54" s="17" t="s">
+      <c r="A54" s="17"/>
+      <c r="B54" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C54" s="17" t="s">
+      <c r="C54" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D54" s="17" t="s">
+      <c r="D54" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E54" s="17" t="s">
+      <c r="E54" s="4" t="s">
         <v>161</v>
       </c>
       <c r="F54" s="10" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
-      <c r="G54" s="17"/>
+      <c r="G54" s="4"/>
     </row>
     <row r="55" spans="1:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="A55" s="39"/>
-      <c r="B55" s="17" t="s">
+      <c r="A55" s="17"/>
+      <c r="B55" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="C55" s="17" t="s">
+      <c r="C55" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D55" s="17" t="s">
+      <c r="D55" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="E55" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="F55" s="32">
+      <c r="E55" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F55" s="24">
         <v>45454</v>
       </c>
-      <c r="G55" s="17"/>
+      <c r="G55" s="4"/>
     </row>
     <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A56" s="39"/>
-      <c r="B56" s="17" t="s">
+      <c r="A56" s="17"/>
+      <c r="B56" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="C56" s="17" t="s">
+      <c r="C56" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D56" s="17" t="s">
+      <c r="D56" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="E56" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="F56" s="32">
+      <c r="E56" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F56" s="24">
         <v>45454</v>
       </c>
-      <c r="G56" s="17"/>
+      <c r="G56" s="4"/>
     </row>
     <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A57" s="39"/>
-      <c r="B57" s="17" t="s">
+      <c r="A57" s="17"/>
+      <c r="B57" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="C57" s="17" t="s">
+      <c r="C57" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D57" s="17" t="s">
+      <c r="D57" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="E57" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="F57" s="32">
+      <c r="E57" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F57" s="24">
         <v>45454</v>
       </c>
-      <c r="G57" s="17"/>
-    </row>
-    <row r="58" spans="1:7" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A58" s="40"/>
-      <c r="B58" s="34" t="s">
+      <c r="G57" s="4"/>
+    </row>
+    <row r="58" spans="1:7" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A58" s="29"/>
+      <c r="B58" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="C58" s="34" t="s">
+      <c r="C58" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="D58" s="34" t="s">
+      <c r="D58" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="E58" s="34" t="s">
+      <c r="E58" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="F58" s="34" t="s">
+      <c r="F58" s="26" t="s">
         <v>188</v>
       </c>
-      <c r="G58" s="34"/>
+      <c r="G58" s="26"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B59" s="4"/>
@@ -8613,11 +10309,11 @@
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="H34:H37"/>
-    <mergeCell ref="A44:A58"/>
     <mergeCell ref="A2:A18"/>
     <mergeCell ref="G2:G4"/>
     <mergeCell ref="A19:A24"/>
     <mergeCell ref="A25:A43"/>
+    <mergeCell ref="A44:A58"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C978">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Oui">
@@ -8628,10 +10324,10 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F16" r:id="rId1" xr:uid="{E755A4D4-7BC0-9C4C-9193-ECD6C6CC1BA7}"/>
-    <hyperlink ref="F17" r:id="rId2" xr:uid="{3C7EF00A-5C01-8C4B-BBDB-C0762AAA5D70}"/>
-    <hyperlink ref="F7" r:id="rId3" xr:uid="{B16E061C-01B2-0341-AB5B-B3E291AC077C}"/>
-    <hyperlink ref="F42" r:id="rId4" xr:uid="{344E3ADC-CA5B-FB4F-8C6D-5B3B87FA69F7}"/>
+    <hyperlink ref="F16" r:id="rId1" xr:uid="{2591B9F9-D9C2-E145-B3EF-CABA271661A8}"/>
+    <hyperlink ref="F17" r:id="rId2" xr:uid="{63B6F830-EEFE-4B41-AEA6-9F81FC68C2E1}"/>
+    <hyperlink ref="F7" r:id="rId3" xr:uid="{2E0649E2-700A-B447-8CC8-C94F1DB3B41A}"/>
+    <hyperlink ref="F42" r:id="rId4" xr:uid="{D58C67B0-4399-7049-B12E-9C91D4137226}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: ajout du code postal de naissance de l'apprenant dans api v3 (#3214)
</commit_message>
<xml_diff>
--- a/ui/public/modele-import.xlsx
+++ b/ui/public/modele-import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raph/dev/flux-retour-cfas/ui/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0B08C7-4D32-4F40-A1A2-A0436210344F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0056733-DBAB-0F4D-88DA-FFFEA358831A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="500" windowWidth="27660" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Modèle" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="216">
   <si>
     <t>ine_apprenant</t>
   </si>
@@ -698,6 +698,15 @@
   </si>
   <si>
     <t>Indiquez OUI (ou VRAI) si le diplôme a été obtenu à l'issue de la formation. Si le diplôme n’a pas été obtenu à l’issue de la formation, indiquez NON (ou FAUX). Si la formation est toujours en cours, ne pas remplir ce champ.</t>
+  </si>
+  <si>
+    <t>code_postal_de_naissance_apprenant</t>
+  </si>
+  <si>
+    <t>code postal du lieu de naissance de l'apprenant</t>
+  </si>
+  <si>
+    <t>5 chiffres</t>
   </si>
 </sst>
 </file>
@@ -1235,7 +1244,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BG2"/>
+  <dimension ref="A1:BH2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -1244,54 +1253,55 @@
     <col min="1" max="1" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="26.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="26.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="30.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="33.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="31.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="35" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="39" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="43" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="48" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="23.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="52" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="24.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="28.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="26" style="1" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="27.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="33.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="34.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="60" max="16384" width="8.83203125" style="1"/>
+    <col min="4" max="4" width="26.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="26.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="26.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="31" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="30.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="33.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="31.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="40" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="44" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="49" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="23.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="53" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="24.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="28.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="26" style="1" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="27.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="33.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="34.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="61" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:60" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>43</v>
       </c>
@@ -1302,175 +1312,178 @@
         <v>56</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="W1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AB1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AC1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AD1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AD1" s="7" t="s">
+      <c r="AE1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AE1" s="7" t="s">
+      <c r="AF1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="AF1" s="7" t="s">
+      <c r="AG1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="AG1" s="7" t="s">
+      <c r="AH1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="AH1" s="7" t="s">
+      <c r="AI1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="AI1" s="7" t="s">
+      <c r="AJ1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="AJ1" s="7" t="s">
+      <c r="AK1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="AK1" s="7" t="s">
+      <c r="AL1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="AL1" s="7" t="s">
+      <c r="AM1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="AM1" s="7" t="s">
+      <c r="AN1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AN1" s="7" t="s">
+      <c r="AO1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AO1" s="7" t="s">
+      <c r="AP1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AP1" s="7" t="s">
+      <c r="AQ1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AQ1" s="7" t="s">
+      <c r="AR1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="AR1" s="7" t="s">
+      <c r="AS1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AS1" s="7" t="s">
+      <c r="AT1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="AT1" s="7" t="s">
+      <c r="AU1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AU1" s="7" t="s">
+      <c r="AV1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="AV1" s="7" t="s">
+      <c r="AW1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="AW1" s="7" t="s">
+      <c r="AX1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="AX1" s="7" t="s">
+      <c r="AY1" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="AY1" s="7" t="s">
+      <c r="AZ1" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="AZ1" s="7" t="s">
+      <c r="BA1" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="BA1" s="7" t="s">
+      <c r="BB1" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="BB1" s="7" t="s">
+      <c r="BC1" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="BC1" s="7" t="s">
+      <c r="BD1" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="BD1" s="7" t="s">
+      <c r="BE1" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="BE1" s="7" t="s">
+      <c r="BF1" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="BF1" s="7" t="s">
+      <c r="BG1" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="BG1" s="7" t="s">
+      <c r="BH1" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:59" s="9" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:60" s="9" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>189</v>
       </c>
@@ -1480,141 +1493,144 @@
       <c r="C2" s="10">
         <v>36827</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="9">
+        <v>44400</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="9">
+      <c r="F2" s="9">
         <v>0</v>
       </c>
-      <c r="F2" s="10">
+      <c r="G2" s="10">
         <v>36827</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="9">
+      <c r="L2" s="9">
         <v>1</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="M2" s="9" t="str">
+      <c r="N2" s="9" t="str">
         <f>"50022141"</f>
         <v>50022141</v>
       </c>
-      <c r="N2" s="10">
+      <c r="O2" s="10">
         <v>44937</v>
-      </c>
-      <c r="O2" s="10">
-        <v>45087</v>
       </c>
       <c r="P2" s="10">
         <v>45087</v>
       </c>
-      <c r="Q2" s="9" t="str">
+      <c r="Q2" s="10">
+        <v>45087</v>
+      </c>
+      <c r="R2" s="9" t="str">
         <f>"1234567890123"</f>
         <v>1234567890123</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="S2" s="9">
+      <c r="T2" s="9">
         <v>44000</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="U2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="U2" s="9" t="b">
+      <c r="V2" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="V2" s="10">
+      <c r="W2" s="10">
         <v>40479</v>
-      </c>
-      <c r="W2" s="9" t="s">
-        <v>40</v>
       </c>
       <c r="X2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="Y2" s="9" t="b">
+      <c r="Y2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z2" s="9" t="b">
         <v>1</v>
-      </c>
-      <c r="Z2" s="10">
-        <v>45087</v>
       </c>
       <c r="AA2" s="10">
         <v>45087</v>
       </c>
-      <c r="AF2" s="9" t="s">
+      <c r="AB2" s="10">
+        <v>45087</v>
+      </c>
+      <c r="AG2" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="AG2" s="10">
+      <c r="AH2" s="10">
         <v>44937</v>
-      </c>
-      <c r="AH2" s="10">
-        <v>45087</v>
       </c>
       <c r="AI2" s="10">
         <v>45087</v>
       </c>
-      <c r="AS2" s="9" t="str">
-        <f>"12345678901235"</f>
-        <v>12345678901235</v>
+      <c r="AJ2" s="10">
+        <v>45087</v>
       </c>
       <c r="AT2" s="9" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
       <c r="AU2" s="9" t="str">
+        <f>"12345678901235"</f>
+        <v>12345678901235</v>
+      </c>
+      <c r="AV2" s="9" t="str">
         <f>"12345678901237"</f>
         <v>12345678901237</v>
       </c>
-      <c r="AV2" s="9" t="str">
+      <c r="AW2" s="9" t="str">
         <f>"12345678901238"</f>
         <v>12345678901238</v>
       </c>
-      <c r="AW2" s="9" t="b">
+      <c r="AX2" s="9" t="b">
         <v>1</v>
-      </c>
-      <c r="AX2" s="10">
-        <v>44937</v>
       </c>
       <c r="AY2" s="10">
         <v>44937</v>
       </c>
       <c r="AZ2" s="10">
+        <v>44937</v>
+      </c>
+      <c r="BA2" s="10">
         <v>45087</v>
       </c>
-      <c r="BA2" s="9">
+      <c r="BB2" s="9">
         <v>4</v>
       </c>
-      <c r="BB2" s="9" t="s">
+      <c r="BC2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="BC2" s="9" t="str">
+      <c r="BD2" s="9" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
-      <c r="BD2" s="9" t="s">
+      <c r="BE2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="BE2" s="9" t="str">
+      <c r="BF2" s="9" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
-      <c r="BF2" s="9" t="s">
+      <c r="BG2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="BG2" s="9" t="str">
+      <c r="BH2" s="9" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
@@ -1627,10 +1643,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587136C3-4E68-704D-AFDE-CEF947822B6E}">
-  <dimension ref="A1:Y977"/>
+  <dimension ref="A1:Y978"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1736,439 +1752,439 @@
         <v>35819</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="27"/>
-      <c r="B5" s="12" t="s">
-        <v>180</v>
+      <c r="B5" s="4" t="s">
+        <v>213</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>58</v>
+        <v>214</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="F5" s="21">
-        <v>35819</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+        <v>215</v>
+      </c>
+      <c r="F5" s="14">
+        <v>44400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27"/>
       <c r="B6" s="12" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>210</v>
+        <v>58</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" ht="45" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+      <c r="F6" s="21">
+        <v>35819</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="27"/>
-      <c r="B7" s="4" t="s">
-        <v>190</v>
+      <c r="B7" s="12" t="s">
+        <v>179</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>157</v>
+        <v>210</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" ht="105" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="F7" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="27"/>
       <c r="B8" s="4" t="s">
-        <v>1</v>
+        <v>190</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>61</v>
+        <v>157</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" ht="60" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="105" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
       <c r="B9" s="4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>63</v>
+        <v>159</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="60" x14ac:dyDescent="0.2">
       <c r="A10" s="27"/>
       <c r="B10" s="4" t="s">
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="60" x14ac:dyDescent="0.2">
+      <c r="A11" s="27"/>
+      <c r="B11" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="4" t="str">
+      <c r="F11" s="4" t="str">
         <f>"1234567890123"</f>
         <v>1234567890123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A11" s="27"/>
-      <c r="B11" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="F11" s="4" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="27"/>
       <c r="B12" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>68</v>
+        <v>161</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="F12" s="21">
-        <v>45160</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" ht="105" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+      <c r="F12" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="27"/>
       <c r="B13" s="4" t="s">
-        <v>191</v>
+        <v>67</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+      <c r="F13" s="21">
+        <v>45160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="105" x14ac:dyDescent="0.2">
       <c r="A14" s="27"/>
       <c r="B14" s="4" t="s">
-        <v>162</v>
+        <v>191</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" s="14">
-        <v>44000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="27"/>
       <c r="B15" s="4" t="s">
-        <v>74</v>
+        <v>162</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>184</v>
+        <v>72</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="14">
+        <v>44000</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="27"/>
       <c r="B16" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="F16" s="15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A17" s="27"/>
+      <c r="B17" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="16" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="17" spans="1:25" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A17" s="28"/>
-      <c r="B17" s="18" t="s">
+    <row r="18" spans="1:25" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A18" s="28"/>
+      <c r="B18" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C18" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D18" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E18" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F18" s="18" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="60" x14ac:dyDescent="0.2">
-      <c r="A18" s="29" t="s">
+    <row r="19" spans="1:25" ht="60" x14ac:dyDescent="0.2">
+      <c r="A19" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" ht="60" x14ac:dyDescent="0.2">
-      <c r="A19" s="27"/>
-      <c r="B19" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F19" s="9" t="str">
-        <f>"12345678901235"</f>
-        <v>12345678901235</v>
+        <v>83</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:25" ht="60" x14ac:dyDescent="0.2">
       <c r="A20" s="27"/>
       <c r="B20" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>41</v>
+        <v>86</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" s="9" t="str">
+        <f>"12345678901235"</f>
+        <v>12345678901235</v>
       </c>
     </row>
     <row r="21" spans="1:25" ht="60" x14ac:dyDescent="0.2">
       <c r="A21" s="27"/>
       <c r="B21" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" ht="60" x14ac:dyDescent="0.2">
+      <c r="A22" s="27"/>
+      <c r="B22" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="F21" s="9" t="str">
+      <c r="F22" s="9" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="45" x14ac:dyDescent="0.2">
-      <c r="A22" s="27"/>
-      <c r="B22" s="4" t="s">
+    <row r="23" spans="1:25" ht="45" x14ac:dyDescent="0.2">
+      <c r="A23" s="27"/>
+      <c r="B23" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E23" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F23" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="60" x14ac:dyDescent="0.2">
-      <c r="A23" s="28"/>
-      <c r="B23" s="5" t="s">
+    <row r="24" spans="1:25" ht="60" x14ac:dyDescent="0.2">
+      <c r="A24" s="28"/>
+      <c r="B24" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C24" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D24" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F23" s="9" t="str">
+      <c r="F24" s="9" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="6"/>
-      <c r="S23" s="6"/>
-      <c r="T23" s="6"/>
-      <c r="U23" s="6"/>
-      <c r="V23" s="6"/>
-      <c r="W23" s="6"/>
-      <c r="X23" s="6"/>
-      <c r="Y23" s="6"/>
-    </row>
-    <row r="24" spans="1:25" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="26" t="s">
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
+      <c r="U24" s="6"/>
+      <c r="V24" s="6"/>
+      <c r="W24" s="6"/>
+      <c r="X24" s="6"/>
+      <c r="Y24" s="6"/>
+    </row>
+    <row r="25" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+      <c r="A25" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F25" s="4" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A25" s="27"/>
-      <c r="B25" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="27"/>
       <c r="B26" s="4" t="s">
-        <v>98</v>
+        <v>193</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="F26" s="22">
-        <v>44832</v>
+        <v>96</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A27" s="27"/>
       <c r="B27" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>182</v>
@@ -2180,13 +2196,13 @@
     <row r="28" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A28" s="27"/>
       <c r="B28" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>182</v>
@@ -2198,103 +2214,103 @@
     <row r="29" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="27"/>
       <c r="B29" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>211</v>
+        <v>103</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="F29" s="4">
-        <v>2</v>
+        <v>182</v>
+      </c>
+      <c r="F29" s="22">
+        <v>44832</v>
       </c>
     </row>
     <row r="30" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" s="27"/>
       <c r="B30" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F30" s="4">
         <v>2</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" ht="45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" s="27"/>
       <c r="B31" s="4" t="s">
-        <v>186</v>
+        <v>2</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>84</v>
+        <v>106</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>107</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" ht="75" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" ht="45" x14ac:dyDescent="0.2">
       <c r="A32" s="27"/>
       <c r="B32" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>166</v>
+        <v>108</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>84</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="33" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" ht="75" x14ac:dyDescent="0.2">
       <c r="A33" s="27"/>
       <c r="B33" s="4" t="s">
-        <v>111</v>
+        <v>187</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>167</v>
+        <v>110</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="F33" s="22">
-        <v>44832</v>
+        <v>166</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="34" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" s="27"/>
       <c r="B34" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>182</v>
@@ -2306,13 +2322,13 @@
     <row r="35" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" s="27"/>
       <c r="B35" s="4" t="s">
-        <v>13</v>
+        <v>112</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>182</v>
@@ -2324,215 +2340,215 @@
     <row r="36" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" s="27"/>
       <c r="B36" s="4" t="s">
-        <v>113</v>
+        <v>13</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="37" spans="1:25" ht="60" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+      <c r="F36" s="22">
+        <v>44832</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A37" s="27"/>
       <c r="B37" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="E37" s="17" t="s">
-        <v>197</v>
-      </c>
-      <c r="F37" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" ht="60" x14ac:dyDescent="0.2">
       <c r="A38" s="27"/>
       <c r="B38" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="F38" s="22">
-        <v>44832</v>
-      </c>
-    </row>
-    <row r="39" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="F38" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" s="27"/>
       <c r="B39" s="4" t="s">
-        <v>15</v>
+        <v>117</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>171</v>
+        <v>118</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>121</v>
+        <v>182</v>
+      </c>
+      <c r="F39" s="22">
+        <v>44832</v>
       </c>
     </row>
     <row r="40" spans="1:25" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="27"/>
       <c r="B40" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>119</v>
+        <v>171</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>120</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="41" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="27"/>
       <c r="B41" s="4" t="s">
-        <v>123</v>
+        <v>16</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D41" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A42" s="27"/>
+      <c r="B42" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E42" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="F41" s="16" t="s">
+      <c r="F42" s="16" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="42" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A42" s="30"/>
-      <c r="B42" s="5" t="s">
+    <row r="43" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A43" s="30"/>
+      <c r="B43" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C43" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D43" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="E42" s="17" t="s">
+      <c r="E43" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="F42" s="18" t="b">
+      <c r="F43" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6"/>
-      <c r="L42" s="6"/>
-      <c r="M42" s="6"/>
-      <c r="N42" s="6"/>
-      <c r="O42" s="6"/>
-      <c r="P42" s="6"/>
-      <c r="Q42" s="6"/>
-      <c r="R42" s="6"/>
-      <c r="S42" s="6"/>
-      <c r="T42" s="6"/>
-      <c r="U42" s="6"/>
-      <c r="V42" s="6"/>
-      <c r="W42" s="6"/>
-      <c r="X42" s="6"/>
-      <c r="Y42" s="6"/>
-    </row>
-    <row r="43" spans="1:25" ht="75" x14ac:dyDescent="0.2">
-      <c r="A43" s="23" t="s">
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
+      <c r="K43" s="6"/>
+      <c r="L43" s="6"/>
+      <c r="M43" s="6"/>
+      <c r="N43" s="6"/>
+      <c r="O43" s="6"/>
+      <c r="P43" s="6"/>
+      <c r="Q43" s="6"/>
+      <c r="R43" s="6"/>
+      <c r="S43" s="6"/>
+      <c r="T43" s="6"/>
+      <c r="U43" s="6"/>
+      <c r="V43" s="6"/>
+      <c r="W43" s="6"/>
+      <c r="X43" s="6"/>
+      <c r="Y43" s="6"/>
+    </row>
+    <row r="44" spans="1:25" ht="75" x14ac:dyDescent="0.2">
+      <c r="A44" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B44" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C44" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D44" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E44" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="F43" s="9" t="str">
+      <c r="F44" s="9" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
-      </c>
-    </row>
-    <row r="44" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A44" s="24"/>
-      <c r="B44" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="F44" s="22">
-        <v>44937</v>
       </c>
     </row>
     <row r="45" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A45" s="24"/>
       <c r="B45" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>182</v>
       </c>
       <c r="F45" s="22">
-        <v>45454</v>
-      </c>
-    </row>
-    <row r="46" spans="1:25" ht="45" x14ac:dyDescent="0.2">
+        <v>44937</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A46" s="24"/>
       <c r="B46" s="4" t="s">
-        <v>132</v>
+        <v>4</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>133</v>
+        <v>60</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>182</v>
@@ -2541,89 +2557,89 @@
         <v>45454</v>
       </c>
     </row>
-    <row r="47" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:25" ht="45" x14ac:dyDescent="0.2">
       <c r="A47" s="24"/>
       <c r="B47" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>60</v>
+        <v>133</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="E47" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="48" spans="1:25" ht="75" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="F47" s="22">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" s="24"/>
       <c r="B48" s="4" t="s">
-        <v>32</v>
+        <v>135</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D48" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+      <c r="A49" s="24"/>
+      <c r="B49" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D49" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="E49" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="F48" s="9" t="str">
+      <c r="F49" s="9" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A49" s="24"/>
-      <c r="B49" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="F49" s="22">
-        <v>44937</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A50" s="24"/>
       <c r="B50" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>182</v>
       </c>
       <c r="F50" s="22">
-        <v>45454</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+        <v>44937</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A51" s="24"/>
-      <c r="B51" s="19" t="s">
-        <v>143</v>
+      <c r="B51" s="4" t="s">
+        <v>141</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>133</v>
+        <v>60</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>182</v>
@@ -2635,68 +2651,68 @@
     <row r="52" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A52" s="24"/>
       <c r="B52" s="19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>60</v>
+        <v>133</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="E52" s="14" t="s">
-        <v>136</v>
+        <v>144</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="F52" s="22">
         <v>45454</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A53" s="24"/>
-      <c r="B53" s="4" t="s">
-        <v>33</v>
+      <c r="B53" s="19" t="s">
+        <v>145</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D53" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="F53" s="22">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+      <c r="A54" s="24"/>
+      <c r="B54" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D54" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="E53" s="4" t="s">
+      <c r="E54" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="F53" s="9" t="str">
+      <c r="F54" s="9" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A54" s="24"/>
-      <c r="B54" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="F54" s="22">
-        <v>45454</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A55" s="24"/>
       <c r="B55" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>182</v>
@@ -2705,16 +2721,16 @@
         <v>45454</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A56" s="24"/>
       <c r="B56" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>133</v>
+        <v>60</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>182</v>
@@ -2723,71 +2739,71 @@
         <v>45454</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A57" s="24"/>
       <c r="B57" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>60</v>
+        <v>133</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+      <c r="F57" s="22">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A58" s="24"/>
       <c r="B58" s="4" t="s">
-        <v>34</v>
+        <v>154</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D58" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+      <c r="A59" s="24"/>
+      <c r="B59" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D59" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="E58" s="4" t="s">
+      <c r="E59" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="F58" s="9" t="str">
+      <c r="F59" s="9" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A59" s="24"/>
-      <c r="B59" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="F59" s="22">
-        <v>45454</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A60" s="24"/>
       <c r="B60" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>182</v>
@@ -2796,16 +2812,16 @@
         <v>45454</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A61" s="24"/>
       <c r="B61" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>133</v>
+        <v>60</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>182</v>
@@ -2814,30 +2830,41 @@
         <v>45454</v>
       </c>
     </row>
-    <row r="62" spans="1:6" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A62" s="25"/>
-      <c r="B62" s="18" t="s">
+    <row r="62" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A62" s="24"/>
+      <c r="B62" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="F62" s="22">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A63" s="25"/>
+      <c r="B63" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="C62" s="18" t="s">
+      <c r="C63" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D62" s="18" t="s">
+      <c r="D63" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="E62" s="18" t="s">
+      <c r="E63" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="F62" s="18" t="s">
+      <c r="F63" s="18" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B64" s="4"/>
@@ -9237,14 +9264,21 @@
       <c r="E977" s="4"/>
       <c r="F977" s="4"/>
     </row>
+    <row r="978" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B978" s="4"/>
+      <c r="C978" s="4"/>
+      <c r="D978" s="4"/>
+      <c r="E978" s="4"/>
+      <c r="F978" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A43:A62"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="A24:A42"/>
+    <mergeCell ref="A44:A63"/>
+    <mergeCell ref="A2:A18"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="A25:A43"/>
   </mergeCells>
-  <conditionalFormatting sqref="C1:C977">
+  <conditionalFormatting sqref="C1:C978">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Oui">
       <formula>NOT(ISERROR(SEARCH(("Oui"),(C1))))</formula>
     </cfRule>
@@ -9253,10 +9287,10 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F15" r:id="rId1" xr:uid="{2591B9F9-D9C2-E145-B3EF-CABA271661A8}"/>
-    <hyperlink ref="F16" r:id="rId2" xr:uid="{63B6F830-EEFE-4B41-AEA6-9F81FC68C2E1}"/>
-    <hyperlink ref="F7" r:id="rId3" xr:uid="{2E0649E2-700A-B447-8CC8-C94F1DB3B41A}"/>
-    <hyperlink ref="F41" r:id="rId4" xr:uid="{D58C67B0-4399-7049-B12E-9C91D4137226}"/>
+    <hyperlink ref="F16" r:id="rId1" xr:uid="{2591B9F9-D9C2-E145-B3EF-CABA271661A8}"/>
+    <hyperlink ref="F17" r:id="rId2" xr:uid="{63B6F830-EEFE-4B41-AEA6-9F81FC68C2E1}"/>
+    <hyperlink ref="F8" r:id="rId3" xr:uid="{2E0649E2-700A-B447-8CC8-C94F1DB3B41A}"/>
+    <hyperlink ref="F42" r:id="rId4" xr:uid="{D58C67B0-4399-7049-B12E-9C91D4137226}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: année scolaire était indiqué comme non obligatoire dans le modèle
</commit_message>
<xml_diff>
--- a/ui/public/modele-import.xlsx
+++ b/ui/public/modele-import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raph/dev/flux-retour-cfas/ui/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0056733-DBAB-0F4D-88DA-FFFEA358831A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCA7997-B95A-4540-AD72-69DCE732DEEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="500" windowWidth="27660" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="215">
   <si>
     <t>ine_apprenant</t>
   </si>
@@ -553,9 +553,6 @@
   </si>
   <si>
     <t xml:space="preserve">UAI du lieu de formation. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">annee_scolaire  </t>
   </si>
   <si>
     <t xml:space="preserve">RNCP + 5 chiffres (RNCPXXXXX) ou 5 chiffre. </t>
@@ -1312,22 +1309,22 @@
         <v>56</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>179</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>180</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>1</v>
@@ -1336,13 +1333,13 @@
         <v>2</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="O1" s="7" t="s">
         <v>3</v>
@@ -1357,13 +1354,13 @@
         <v>6</v>
       </c>
       <c r="S1" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="T1" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>195</v>
-      </c>
-      <c r="U1" s="7" t="s">
-        <v>196</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>7</v>
@@ -1456,13 +1453,13 @@
         <v>98</v>
       </c>
       <c r="AZ1" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="BA1" s="7" t="s">
         <v>102</v>
       </c>
       <c r="BB1" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="BC1" s="7" t="s">
         <v>82</v>
@@ -1485,7 +1482,7 @@
     </row>
     <row r="2" spans="1:60" s="9" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>36</v>
@@ -1506,13 +1503,13 @@
         <v>36827</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>37</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>38</v>
@@ -1521,7 +1518,7 @@
         <v>1</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N2" s="9" t="str">
         <f>"50022141"</f>
@@ -1571,7 +1568,7 @@
         <v>45087</v>
       </c>
       <c r="AG2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AH2" s="10">
         <v>44937</v>
@@ -1645,8 +1642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587136C3-4E68-704D-AFDE-CEF947822B6E}">
   <dimension ref="A1:Y978"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1746,7 +1743,7 @@
         <v>57</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F4" s="21">
         <v>35819</v>
@@ -1755,16 +1752,16 @@
     <row r="5" spans="1:25" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="27"/>
       <c r="B5" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>214</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>215</v>
       </c>
       <c r="F5" s="14">
         <v>44400</v>
@@ -1773,7 +1770,7 @@
     <row r="6" spans="1:25" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27"/>
       <c r="B6" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>51</v>
@@ -1782,7 +1779,7 @@
         <v>58</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F6" s="21">
         <v>35819</v>
@@ -1791,13 +1788,13 @@
     <row r="7" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="27"/>
       <c r="B7" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>59</v>
@@ -1809,7 +1806,7 @@
     <row r="8" spans="1:25" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="27"/>
       <c r="B8" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>51</v>
@@ -1839,7 +1836,7 @@
         <v>159</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="60" x14ac:dyDescent="0.2">
@@ -1857,7 +1854,7 @@
         <v>63</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="60" x14ac:dyDescent="0.2">
@@ -1891,7 +1888,7 @@
         <v>161</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F12" s="4" t="b">
         <v>1</v>
@@ -1909,7 +1906,7 @@
         <v>68</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F13" s="21">
         <v>45160</v>
@@ -1918,7 +1915,7 @@
     <row r="14" spans="1:25" ht="105" x14ac:dyDescent="0.2">
       <c r="A14" s="27"/>
       <c r="B14" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>51</v>
@@ -1966,7 +1963,7 @@
         <v>76</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="30" x14ac:dyDescent="0.2">
@@ -1984,13 +1981,13 @@
         <v>76</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" spans="1:25" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A18" s="28"/>
       <c r="B18" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C18" s="18" t="s">
         <v>51</v>
@@ -2142,10 +2139,10 @@
         <v>92</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>93</v>
@@ -2160,7 +2157,7 @@
     <row r="26" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="27"/>
       <c r="B26" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>51</v>
@@ -2187,7 +2184,7 @@
         <v>99</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F27" s="22">
         <v>44832</v>
@@ -2205,7 +2202,7 @@
         <v>101</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F28" s="22">
         <v>44832</v>
@@ -2223,7 +2220,7 @@
         <v>103</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F29" s="22">
         <v>44832</v>
@@ -2238,7 +2235,7 @@
         <v>51</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>105</v>
@@ -2268,7 +2265,7 @@
     <row r="32" spans="1:25" ht="45" x14ac:dyDescent="0.2">
       <c r="A32" s="27"/>
       <c r="B32" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>51</v>
@@ -2286,7 +2283,7 @@
     <row r="33" spans="1:25" ht="75" x14ac:dyDescent="0.2">
       <c r="A33" s="27"/>
       <c r="B33" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>51</v>
@@ -2295,10 +2292,10 @@
         <v>110</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="34" spans="1:25" ht="30" x14ac:dyDescent="0.2">
@@ -2310,10 +2307,10 @@
         <v>60</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F34" s="22">
         <v>44832</v>
@@ -2328,10 +2325,10 @@
         <v>60</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F35" s="22">
         <v>44832</v>
@@ -2346,10 +2343,10 @@
         <v>60</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F36" s="22">
         <v>44832</v>
@@ -2364,7 +2361,7 @@
         <v>60</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>114</v>
@@ -2382,10 +2379,10 @@
         <v>60</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F38" s="4" t="b">
         <v>1</v>
@@ -2403,7 +2400,7 @@
         <v>118</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F39" s="22">
         <v>44832</v>
@@ -2418,7 +2415,7 @@
         <v>60</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>120</v>
@@ -2454,13 +2451,13 @@
         <v>60</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>124</v>
       </c>
       <c r="F42" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="43" spans="1:25" ht="30" x14ac:dyDescent="0.2">
@@ -2472,10 +2469,10 @@
         <v>60</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E43" s="17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F43" s="18" t="b">
         <v>1</v>
@@ -2508,7 +2505,7 @@
         <v>127</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>128</v>
@@ -2533,7 +2530,7 @@
         <v>130</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F45" s="22">
         <v>44937</v>
@@ -2551,7 +2548,7 @@
         <v>131</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F46" s="22">
         <v>45454</v>
@@ -2569,7 +2566,7 @@
         <v>134</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F47" s="22">
         <v>45454</v>
@@ -2584,7 +2581,7 @@
         <v>60</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E48" s="14" t="s">
         <v>136</v>
@@ -2624,7 +2621,7 @@
         <v>140</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F50" s="22">
         <v>44937</v>
@@ -2642,7 +2639,7 @@
         <v>142</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F51" s="22">
         <v>45454</v>
@@ -2660,7 +2657,7 @@
         <v>144</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F52" s="22">
         <v>45454</v>
@@ -2715,7 +2712,7 @@
         <v>149</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F55" s="22">
         <v>45454</v>
@@ -2733,7 +2730,7 @@
         <v>151</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F56" s="22">
         <v>45454</v>
@@ -2751,7 +2748,7 @@
         <v>153</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F57" s="22">
         <v>45454</v>
@@ -2784,7 +2781,7 @@
         <v>60</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>129</v>
@@ -2797,16 +2794,16 @@
     <row r="60" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A60" s="24"/>
       <c r="B60" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F60" s="22">
         <v>45454</v>
@@ -2815,16 +2812,16 @@
     <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A61" s="24"/>
       <c r="B61" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F61" s="22">
         <v>45454</v>
@@ -2833,16 +2830,16 @@
     <row r="62" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A62" s="24"/>
       <c r="B62" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>133</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F62" s="22">
         <v>45454</v>
@@ -2851,13 +2848,13 @@
     <row r="63" spans="1:6" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A63" s="25"/>
       <c r="B63" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C63" s="18" t="s">
         <v>60</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E63" s="18" t="s">
         <v>107</v>

</xml_diff>

<commit_message>
chore: update excel modele
</commit_message>
<xml_diff>
--- a/ui/public/modele-import.xlsx
+++ b/ui/public/modele-import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raph/dev/flux-retour-cfas/ui/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39528BFA-4694-5041-B7F4-45B109D29572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25C40EE-7344-ED4A-8271-3EE29CB38492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="500" windowWidth="27660" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -204,9 +204,6 @@
     <t>date_fin_formation *</t>
   </si>
   <si>
-    <t>duree_theorique_formation *</t>
-  </si>
-  <si>
     <t>etablissement_responsable_uai *</t>
   </si>
   <si>
@@ -457,12 +454,6 @@
     <t>date de fin prévisionnelle de la formation</t>
   </si>
   <si>
-    <t>Durée théorique de la formation, de la date d'inscription au diplôme, exprimée en années.</t>
-  </si>
-  <si>
-    <t>minimum : 1 / minimum 4</t>
-  </si>
-  <si>
     <t>Libellé court de la formation</t>
   </si>
   <si>
@@ -653,6 +644,15 @@
   </si>
   <si>
     <t>Il s’agit du code UAI de l’établissement qui accueille physiquement et forme l'apprenant. Il ne correspond pas nécessairement à l’établissement responsable de la gestion de la  formation. Si l’apprenant est formé au sein de l’établissement responsable de la gestion de la formation, indiquez le même UAI et SIRET.</t>
+  </si>
+  <si>
+    <t>Durée théorique de la formation, de la date d'inscription au diplôme, exprimée en mois.</t>
+  </si>
+  <si>
+    <t>minimum : 1 / maximum 48</t>
+  </si>
+  <si>
+    <t>duree_theorique_formation_mois *</t>
   </si>
 </sst>
 </file>
@@ -837,7 +837,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -864,30 +864,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -921,10 +897,33 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1354,7 +1353,7 @@
     <col min="30" max="30" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="21.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="25.5" style="1" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="21.5" style="1" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="25.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -1443,22 +1442,22 @@
         <v>26</v>
       </c>
       <c r="T1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U1" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="W1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="Y1" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="Z1" s="9" t="s">
         <v>4</v>
@@ -1482,7 +1481,7 @@
         <v>54</v>
       </c>
       <c r="AG1" s="9" t="s">
-        <v>55</v>
+        <v>196</v>
       </c>
       <c r="AH1" s="9" t="s">
         <v>10</v>
@@ -1574,10 +1573,10 @@
     </row>
     <row r="2" spans="1:62" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
@@ -1589,29 +1588,29 @@
         <v>36827</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G2" s="2">
         <v>44400</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J2" s="2">
         <v>44000</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L2" s="2" t="str">
         <f>"1234567890123"</f>
         <v>1234567890123</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N2" s="2" t="b">
         <f>TRUE()</f>
@@ -1621,46 +1620,46 @@
         <v>40479</v>
       </c>
       <c r="P2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="S2" s="2">
         <v>4101</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U2" s="2" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W2" s="2" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Y2" s="2" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AA2" s="2">
         <v>1</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AC2" s="2" t="str">
         <f>"50022141"</f>
@@ -1676,10 +1675,10 @@
         <v>45087</v>
       </c>
       <c r="AG2" s="2">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AI2" s="2" t="b">
         <f>TRUE()</f>
@@ -1709,7 +1708,7 @@
         <v>45087</v>
       </c>
       <c r="AU2" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AV2" s="3">
         <v>44937</v>
@@ -1743,8 +1742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y978"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A20"/>
+    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1759,350 +1758,350 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="34"/>
-      <c r="B1" s="35" t="s">
+      <c r="A1" s="25"/>
+      <c r="B1" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="D1" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="E1" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="F1" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+    </row>
+    <row r="2" spans="1:25" ht="60" x14ac:dyDescent="0.2">
+      <c r="A2" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-    </row>
-    <row r="2" spans="1:25" ht="60" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="B2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="21" t="s">
+      <c r="D2" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="E2" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="F2" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="F2" s="21" t="s">
+    </row>
+    <row r="3" spans="1:25" ht="60" x14ac:dyDescent="0.2">
+      <c r="A3" s="27"/>
+      <c r="B3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" ht="60" x14ac:dyDescent="0.2">
-      <c r="A3" s="12"/>
-      <c r="B3" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D3" s="21" t="s">
+      <c r="E3" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" s="27"/>
+      <c r="B4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
-      <c r="B4" s="21" t="s">
+      <c r="E4" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="18">
+        <v>35819</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="27"/>
+      <c r="B5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="15">
+        <v>44400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="27"/>
+      <c r="B6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" s="18">
+        <v>35819</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A7" s="27"/>
+      <c r="B7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" s="13">
         <v>2</v>
       </c>
-      <c r="C4" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="E4" s="21" t="s">
+    </row>
+    <row r="8" spans="1:25" ht="45" x14ac:dyDescent="0.2">
+      <c r="A8" s="27"/>
+      <c r="B8" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="105" x14ac:dyDescent="0.2">
+      <c r="A9" s="27"/>
+      <c r="B9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F4" s="26">
-        <v>35819</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="12"/>
-      <c r="B5" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="F5" s="23">
-        <v>44400</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12"/>
-      <c r="B6" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="E6" s="21" t="s">
+      <c r="D9" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="45" x14ac:dyDescent="0.2">
+      <c r="A10" s="27"/>
+      <c r="B10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F6" s="26">
-        <v>35819</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
-      <c r="B7" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="F7" s="21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" ht="45" x14ac:dyDescent="0.2">
-      <c r="A8" s="12"/>
-      <c r="B8" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="F8" s="27" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" ht="105" x14ac:dyDescent="0.2">
-      <c r="A9" s="12"/>
-      <c r="B9" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="F9" s="21" t="s">
+      <c r="D10" s="13" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" ht="45" x14ac:dyDescent="0.2">
-      <c r="A10" s="12"/>
-      <c r="B10" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D10" s="21" t="s">
+      <c r="E10" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="F10" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="60" x14ac:dyDescent="0.2">
+      <c r="A11" s="27"/>
+      <c r="B11" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="F10" s="21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" ht="60" x14ac:dyDescent="0.2">
-      <c r="A11" s="12"/>
-      <c r="B11" s="21" t="s">
+      <c r="C11" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D11" s="21" t="s">
+      <c r="E11" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="F11" s="21" t="str">
+      <c r="F11" s="13" t="str">
         <f>"1234567890123"</f>
         <v>1234567890123</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
-      <c r="B12" s="21" t="s">
+      <c r="A12" s="27"/>
+      <c r="B12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D12" s="21" t="s">
+      <c r="C12" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="E12" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="F12" s="21" t="b">
+      <c r="F12" s="13" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A13" s="12"/>
-      <c r="B13" s="21" t="s">
+      <c r="A13" s="27"/>
+      <c r="B13" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D13" s="21" t="s">
+      <c r="C13" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="18">
+        <v>45160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="105" x14ac:dyDescent="0.2">
+      <c r="A14" s="27"/>
+      <c r="B14" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E14" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="27"/>
+      <c r="B15" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" s="15">
+        <v>44000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A16" s="27"/>
+      <c r="B16" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F13" s="26">
-        <v>45160</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" ht="105" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
-      <c r="B14" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
-      <c r="B15" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="E15" s="28" t="s">
+      <c r="D16" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="F15" s="23">
-        <v>44000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
-      <c r="B16" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D16" s="21" t="s">
+      <c r="E16" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="F16" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="F16" s="29" t="s">
+    </row>
+    <row r="17" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A17" s="27"/>
+      <c r="B17" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="13" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A17" s="12"/>
-      <c r="B17" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D17" s="21" t="s">
+      <c r="E17" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="F17" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="E17" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="F17" s="27" t="s">
+    </row>
+    <row r="18" spans="1:25" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A18" s="27"/>
+      <c r="B18" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="13" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="18" spans="1:25" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
-      <c r="B18" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D18" s="21" t="s">
+      <c r="E18" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="F18" s="15" t="s">
         <v>117</v>
-      </c>
-      <c r="F18" s="23" t="s">
-        <v>118</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
@@ -2125,773 +2124,773 @@
       <c r="Y18" s="4"/>
     </row>
     <row r="19" spans="1:25" ht="45" x14ac:dyDescent="0.2">
-      <c r="A19" s="12"/>
-      <c r="B19" s="21" t="s">
+      <c r="A19" s="27"/>
+      <c r="B19" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" s="21" t="s">
+      <c r="C19" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="F19" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="A20" s="27"/>
+      <c r="B20" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="F19" s="23" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A20" s="12"/>
-      <c r="B20" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="D20" s="24" t="s">
+      <c r="E20" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="F20" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="F20" s="24" t="s">
+    </row>
+    <row r="21" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="28" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="21" spans="1:25" s="33" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="13" t="s">
+      <c r="B21" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" ht="60" x14ac:dyDescent="0.2">
+      <c r="A22" s="29"/>
+      <c r="B22" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="B21" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="F21" s="21" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" ht="60" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D22" s="21" t="s">
+      <c r="E22" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="E22" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="F22" s="22" t="str">
+      <c r="F22" s="14" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
     </row>
     <row r="23" spans="1:25" ht="75" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
-      <c r="B23" s="21" t="s">
+      <c r="A23" s="29"/>
+      <c r="B23" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" ht="60" x14ac:dyDescent="0.2">
+      <c r="A24" s="29"/>
+      <c r="B24" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>196</v>
-      </c>
-      <c r="E23" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="F23" s="21" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" ht="60" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
-      <c r="B24" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="21" t="s">
+      <c r="C24" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E24" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="E24" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="F24" s="22" t="str">
+      <c r="F24" s="14" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
     </row>
     <row r="25" spans="1:25" ht="90" x14ac:dyDescent="0.2">
-      <c r="A25" s="14"/>
-      <c r="B25" s="21" t="s">
+      <c r="A25" s="29"/>
+      <c r="B25" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="A26" s="30"/>
+      <c r="B26" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>195</v>
-      </c>
-      <c r="E25" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="F25" s="21" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A26" s="15"/>
-      <c r="B26" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="D26" s="24" t="s">
+      <c r="C26" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="E26" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="E26" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="F26" s="25" t="str">
+      <c r="F26" s="17" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
     </row>
     <row r="27" spans="1:25" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="B27" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D27" s="21" t="s">
+      <c r="E27" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="F27" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A28" s="31"/>
+      <c r="B28" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="F27" s="21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A28" s="16"/>
-      <c r="B28" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D28" s="21" t="s">
+      <c r="E28" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="F28" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="F28" s="23" t="s">
+    </row>
+    <row r="29" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A29" s="31"/>
+      <c r="B29" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="13" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="29" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A29" s="16"/>
-      <c r="B29" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D29" s="21" t="s">
+      <c r="E29" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F29" s="22">
+        <v>44832</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A30" s="31"/>
+      <c r="B30" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="E29" s="21" t="s">
+      <c r="E30" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30" s="22">
+        <v>44832</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A31" s="31"/>
+      <c r="B31" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F31" s="22">
+        <v>44832</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A32" s="31"/>
+      <c r="B32" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="F32" s="13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A33" s="31"/>
+      <c r="B33" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F29" s="30">
+      <c r="D33" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A34" s="31"/>
+      <c r="B34" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+      <c r="A35" s="31"/>
+      <c r="B35" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A36" s="31"/>
+      <c r="B36" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F36" s="22">
         <v>44832</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A30" s="16"/>
-      <c r="B30" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="E30" s="21" t="s">
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A37" s="31"/>
+      <c r="B37" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="C37" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F30" s="30">
-        <v>44832</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A31" s="16"/>
-      <c r="B31" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D31" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="E31" s="21" t="s">
+      <c r="D37" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A38" s="31"/>
+      <c r="B38" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F31" s="30">
-        <v>44832</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A32" s="16"/>
-      <c r="B32" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D32" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="E32" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="F32" s="21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A33" s="16"/>
-      <c r="B33" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D33" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="E33" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="F33" s="21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A34" s="16"/>
-      <c r="B34" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="C34" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D34" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="E34" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="F34" s="21" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="75" x14ac:dyDescent="0.2">
-      <c r="A35" s="16"/>
-      <c r="B35" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="C35" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D35" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="E35" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="F35" s="21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A36" s="16"/>
-      <c r="B36" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D36" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="E36" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="F36" s="30">
-        <v>44832</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A37" s="16"/>
-      <c r="B37" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="C37" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D37" s="21" t="s">
+      <c r="D38" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="E37" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="F37" s="21" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="60" x14ac:dyDescent="0.2">
-      <c r="A38" s="16"/>
-      <c r="B38" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C38" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D38" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="E38" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="F38" s="21" t="b">
+      <c r="E38" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="F38" s="13" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A39" s="16"/>
-      <c r="B39" s="21" t="s">
+      <c r="A39" s="31"/>
+      <c r="B39" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D39" s="21" t="s">
+      <c r="C39" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F39" s="22">
+        <v>44832</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A40" s="31"/>
+      <c r="B40" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="F40" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="E39" s="21" t="s">
+    </row>
+    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A41" s="31"/>
+      <c r="B41" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F39" s="30">
-        <v>44832</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A40" s="16"/>
-      <c r="B40" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D40" s="21" t="s">
+      <c r="D41" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="E40" s="21" t="s">
+      <c r="E41" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="F41" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="F40" s="21" t="s">
+    </row>
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A42" s="31"/>
+      <c r="B42" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="E42" s="13" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A41" s="16"/>
-      <c r="B41" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C41" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D41" s="21" t="s">
+      <c r="F42" s="19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A43" s="31"/>
+      <c r="B43" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="E41" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="F41" s="21" t="s">
+      <c r="C43" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" s="13" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A42" s="16"/>
-      <c r="B42" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C42" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D42" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="E42" s="21" t="s">
-        <v>158</v>
-      </c>
-      <c r="F42" s="27" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A43" s="16"/>
-      <c r="B43" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="C43" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D43" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="E43" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="F43" s="21" t="b">
+      <c r="E43" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="F43" s="13" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="11" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="17" t="s">
+      <c r="A44" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="E44" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="B44" s="20" t="s">
-        <v>190</v>
-      </c>
-      <c r="C44" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="D44" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="E44" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="F44" s="31" t="str">
+      <c r="F44" s="23" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A45" s="18"/>
-      <c r="B45" s="21" t="s">
+      <c r="A45" s="33"/>
+      <c r="B45" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C45" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D45" s="21" t="s">
+      <c r="C45" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F45" s="22">
+        <v>44937</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A46" s="33"/>
+      <c r="B46" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F46" s="22">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A47" s="33"/>
+      <c r="B47" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="C47" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="E45" s="21" t="s">
+      <c r="D47" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F47" s="22">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A48" s="33"/>
+      <c r="B48" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="C48" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F45" s="30">
-        <v>44937</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A46" s="18"/>
-      <c r="B46" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C46" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D46" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="E46" s="21" t="s">
+      <c r="D48" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25" ht="75" x14ac:dyDescent="0.2">
+      <c r="A49" s="33"/>
+      <c r="B49" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F46" s="30">
-        <v>45454</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A47" s="18"/>
-      <c r="B47" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="C47" s="21" t="s">
-        <v>168</v>
-      </c>
-      <c r="D47" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E47" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="F47" s="30">
-        <v>45454</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A48" s="18"/>
-      <c r="B48" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="C48" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D48" s="21" t="s">
+      <c r="D49" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="E48" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="F48" s="21" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="49" spans="1:25" ht="75" x14ac:dyDescent="0.2">
-      <c r="A49" s="18"/>
-      <c r="B49" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C49" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D49" s="21" t="s">
-        <v>173</v>
-      </c>
-      <c r="E49" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="F49" s="22" t="str">
+      <c r="E49" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="F49" s="14" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
     </row>
     <row r="50" spans="1:25" ht="45" x14ac:dyDescent="0.2">
-      <c r="A50" s="18"/>
-      <c r="B50" s="21" t="s">
+      <c r="A50" s="33"/>
+      <c r="B50" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C50" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D50" s="21" t="s">
+      <c r="C50" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="E50" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F50" s="22">
+        <v>44937</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25" ht="45" x14ac:dyDescent="0.2">
+      <c r="A51" s="33"/>
+      <c r="B51" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F51" s="22">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A52" s="33"/>
+      <c r="B52" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C52" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="D52" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F52" s="22">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A53" s="33"/>
+      <c r="B53" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="C53" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D53" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="E50" s="21" t="s">
+      <c r="E53" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="F53" s="22">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25" ht="75" x14ac:dyDescent="0.2">
+      <c r="A54" s="33"/>
+      <c r="B54" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C54" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F50" s="30">
-        <v>44937</v>
-      </c>
-    </row>
-    <row r="51" spans="1:25" ht="45" x14ac:dyDescent="0.2">
-      <c r="A51" s="18"/>
-      <c r="B51" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C51" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D51" s="21" t="s">
+      <c r="D54" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="E51" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="F51" s="30">
-        <v>45454</v>
-      </c>
-    </row>
-    <row r="52" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A52" s="18"/>
-      <c r="B52" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="C52" s="32" t="s">
-        <v>168</v>
-      </c>
-      <c r="D52" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="E52" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="F52" s="30">
-        <v>45454</v>
-      </c>
-    </row>
-    <row r="53" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A53" s="18"/>
-      <c r="B53" s="21" t="s">
-        <v>192</v>
-      </c>
-      <c r="C53" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="D53" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="E53" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="F53" s="30">
-        <v>45454</v>
-      </c>
-    </row>
-    <row r="54" spans="1:25" ht="75" x14ac:dyDescent="0.2">
-      <c r="A54" s="18"/>
-      <c r="B54" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C54" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D54" s="21" t="s">
-        <v>178</v>
-      </c>
-      <c r="E54" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="F54" s="22" t="str">
+      <c r="E54" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="F54" s="14" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
     </row>
     <row r="55" spans="1:25" ht="45" x14ac:dyDescent="0.2">
-      <c r="A55" s="18"/>
-      <c r="B55" s="21" t="s">
+      <c r="A55" s="33"/>
+      <c r="B55" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C55" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D55" s="21" t="s">
+      <c r="C55" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D55" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="E55" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F55" s="22">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="56" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A56" s="33"/>
+      <c r="B56" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D56" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="E56" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F56" s="22">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="57" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A57" s="33"/>
+      <c r="B57" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="D57" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="E57" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F57" s="22">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="58" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A58" s="33"/>
+      <c r="B58" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D58" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="E55" s="21" t="s">
+      <c r="E58" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F58" s="13" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25" ht="75" x14ac:dyDescent="0.2">
+      <c r="A59" s="33"/>
+      <c r="B59" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C59" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F55" s="30">
-        <v>45454</v>
-      </c>
-    </row>
-    <row r="56" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A56" s="18"/>
-      <c r="B56" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C56" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D56" s="21" t="s">
-        <v>180</v>
-      </c>
-      <c r="E56" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="F56" s="30">
-        <v>45454</v>
-      </c>
-    </row>
-    <row r="57" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A57" s="18"/>
-      <c r="B57" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C57" s="21" t="s">
-        <v>168</v>
-      </c>
-      <c r="D57" s="21" t="s">
+      <c r="D59" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="E57" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="F57" s="30">
-        <v>45454</v>
-      </c>
-    </row>
-    <row r="58" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A58" s="18"/>
-      <c r="B58" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="C58" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D58" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="E58" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="F58" s="21" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="59" spans="1:25" ht="75" x14ac:dyDescent="0.2">
-      <c r="A59" s="18"/>
-      <c r="B59" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C59" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D59" s="21" t="s">
-        <v>184</v>
-      </c>
-      <c r="E59" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="F59" s="22" t="str">
+      <c r="E59" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="F59" s="14" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
     </row>
     <row r="60" spans="1:25" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A60" s="18"/>
-      <c r="B60" s="21" t="s">
+      <c r="A60" s="33"/>
+      <c r="B60" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C60" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D60" s="21" t="s">
-        <v>185</v>
-      </c>
-      <c r="E60" s="21" t="s">
+      <c r="C60" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F60" s="30">
+      <c r="D60" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="E60" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F60" s="22">
         <v>45454</v>
       </c>
       <c r="G60" s="4"/>
@@ -2915,57 +2914,57 @@
       <c r="Y60" s="4"/>
     </row>
     <row r="61" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A61" s="18"/>
-      <c r="B61" s="21" t="s">
+      <c r="A61" s="33"/>
+      <c r="B61" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C61" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D61" s="21" t="s">
-        <v>186</v>
-      </c>
-      <c r="E61" s="21" t="s">
+      <c r="C61" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F61" s="30">
+      <c r="D61" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="E61" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F61" s="22">
         <v>45454</v>
       </c>
     </row>
     <row r="62" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A62" s="18"/>
-      <c r="B62" s="21" t="s">
+      <c r="A62" s="33"/>
+      <c r="B62" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C62" s="21" t="s">
-        <v>168</v>
-      </c>
-      <c r="D62" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="E62" s="21" t="s">
+      <c r="C62" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="D62" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="E62" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F62" s="22">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="63" spans="1:25" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A63" s="34"/>
+      <c r="B63" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C63" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="F62" s="30">
-        <v>45454</v>
-      </c>
-    </row>
-    <row r="63" spans="1:25" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A63" s="19"/>
-      <c r="B63" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C63" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="D63" s="24" t="s">
-        <v>188</v>
-      </c>
-      <c r="E63" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="F63" s="24" t="s">
-        <v>183</v>
+      <c r="D63" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="E63" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="F63" s="16" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feat: ajout de la durée théorique en mois, rétrocompatible et le système en année fonctionne encore (#3394)
</commit_message>
<xml_diff>
--- a/ui/public/modele-import.xlsx
+++ b/ui/public/modele-import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raph/dev/flux-retour-cfas/ui/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39528BFA-4694-5041-B7F4-45B109D29572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25C40EE-7344-ED4A-8271-3EE29CB38492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="500" windowWidth="27660" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -204,9 +204,6 @@
     <t>date_fin_formation *</t>
   </si>
   <si>
-    <t>duree_theorique_formation *</t>
-  </si>
-  <si>
     <t>etablissement_responsable_uai *</t>
   </si>
   <si>
@@ -457,12 +454,6 @@
     <t>date de fin prévisionnelle de la formation</t>
   </si>
   <si>
-    <t>Durée théorique de la formation, de la date d'inscription au diplôme, exprimée en années.</t>
-  </si>
-  <si>
-    <t>minimum : 1 / minimum 4</t>
-  </si>
-  <si>
     <t>Libellé court de la formation</t>
   </si>
   <si>
@@ -653,6 +644,15 @@
   </si>
   <si>
     <t>Il s’agit du code UAI de l’établissement qui accueille physiquement et forme l'apprenant. Il ne correspond pas nécessairement à l’établissement responsable de la gestion de la  formation. Si l’apprenant est formé au sein de l’établissement responsable de la gestion de la formation, indiquez le même UAI et SIRET.</t>
+  </si>
+  <si>
+    <t>Durée théorique de la formation, de la date d'inscription au diplôme, exprimée en mois.</t>
+  </si>
+  <si>
+    <t>minimum : 1 / maximum 48</t>
+  </si>
+  <si>
+    <t>duree_theorique_formation_mois *</t>
   </si>
 </sst>
 </file>
@@ -837,7 +837,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -864,30 +864,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -921,10 +897,33 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1354,7 +1353,7 @@
     <col min="30" max="30" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="21.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="25.5" style="1" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="21.5" style="1" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="25.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -1443,22 +1442,22 @@
         <v>26</v>
       </c>
       <c r="T1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U1" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="W1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="Y1" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="Z1" s="9" t="s">
         <v>4</v>
@@ -1482,7 +1481,7 @@
         <v>54</v>
       </c>
       <c r="AG1" s="9" t="s">
-        <v>55</v>
+        <v>196</v>
       </c>
       <c r="AH1" s="9" t="s">
         <v>10</v>
@@ -1574,10 +1573,10 @@
     </row>
     <row r="2" spans="1:62" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
@@ -1589,29 +1588,29 @@
         <v>36827</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G2" s="2">
         <v>44400</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J2" s="2">
         <v>44000</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L2" s="2" t="str">
         <f>"1234567890123"</f>
         <v>1234567890123</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N2" s="2" t="b">
         <f>TRUE()</f>
@@ -1621,46 +1620,46 @@
         <v>40479</v>
       </c>
       <c r="P2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="S2" s="2">
         <v>4101</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U2" s="2" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W2" s="2" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Y2" s="2" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AA2" s="2">
         <v>1</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AC2" s="2" t="str">
         <f>"50022141"</f>
@@ -1676,10 +1675,10 @@
         <v>45087</v>
       </c>
       <c r="AG2" s="2">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AI2" s="2" t="b">
         <f>TRUE()</f>
@@ -1709,7 +1708,7 @@
         <v>45087</v>
       </c>
       <c r="AU2" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AV2" s="3">
         <v>44937</v>
@@ -1743,8 +1742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y978"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A20"/>
+    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1759,350 +1758,350 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="34"/>
-      <c r="B1" s="35" t="s">
+      <c r="A1" s="25"/>
+      <c r="B1" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="D1" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="E1" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="F1" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+    </row>
+    <row r="2" spans="1:25" ht="60" x14ac:dyDescent="0.2">
+      <c r="A2" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-    </row>
-    <row r="2" spans="1:25" ht="60" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="B2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="21" t="s">
+      <c r="D2" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="E2" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="F2" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="F2" s="21" t="s">
+    </row>
+    <row r="3" spans="1:25" ht="60" x14ac:dyDescent="0.2">
+      <c r="A3" s="27"/>
+      <c r="B3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" ht="60" x14ac:dyDescent="0.2">
-      <c r="A3" s="12"/>
-      <c r="B3" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D3" s="21" t="s">
+      <c r="E3" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" s="27"/>
+      <c r="B4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
-      <c r="B4" s="21" t="s">
+      <c r="E4" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="18">
+        <v>35819</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="27"/>
+      <c r="B5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="15">
+        <v>44400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="27"/>
+      <c r="B6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" s="18">
+        <v>35819</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A7" s="27"/>
+      <c r="B7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" s="13">
         <v>2</v>
       </c>
-      <c r="C4" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="E4" s="21" t="s">
+    </row>
+    <row r="8" spans="1:25" ht="45" x14ac:dyDescent="0.2">
+      <c r="A8" s="27"/>
+      <c r="B8" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="105" x14ac:dyDescent="0.2">
+      <c r="A9" s="27"/>
+      <c r="B9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F4" s="26">
-        <v>35819</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="12"/>
-      <c r="B5" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="F5" s="23">
-        <v>44400</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12"/>
-      <c r="B6" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="E6" s="21" t="s">
+      <c r="D9" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="45" x14ac:dyDescent="0.2">
+      <c r="A10" s="27"/>
+      <c r="B10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F6" s="26">
-        <v>35819</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
-      <c r="B7" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="F7" s="21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" ht="45" x14ac:dyDescent="0.2">
-      <c r="A8" s="12"/>
-      <c r="B8" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="F8" s="27" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" ht="105" x14ac:dyDescent="0.2">
-      <c r="A9" s="12"/>
-      <c r="B9" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="F9" s="21" t="s">
+      <c r="D10" s="13" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" ht="45" x14ac:dyDescent="0.2">
-      <c r="A10" s="12"/>
-      <c r="B10" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D10" s="21" t="s">
+      <c r="E10" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="F10" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="60" x14ac:dyDescent="0.2">
+      <c r="A11" s="27"/>
+      <c r="B11" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="F10" s="21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" ht="60" x14ac:dyDescent="0.2">
-      <c r="A11" s="12"/>
-      <c r="B11" s="21" t="s">
+      <c r="C11" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D11" s="21" t="s">
+      <c r="E11" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="F11" s="21" t="str">
+      <c r="F11" s="13" t="str">
         <f>"1234567890123"</f>
         <v>1234567890123</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
-      <c r="B12" s="21" t="s">
+      <c r="A12" s="27"/>
+      <c r="B12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D12" s="21" t="s">
+      <c r="C12" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="E12" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="F12" s="21" t="b">
+      <c r="F12" s="13" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A13" s="12"/>
-      <c r="B13" s="21" t="s">
+      <c r="A13" s="27"/>
+      <c r="B13" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D13" s="21" t="s">
+      <c r="C13" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="18">
+        <v>45160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="105" x14ac:dyDescent="0.2">
+      <c r="A14" s="27"/>
+      <c r="B14" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E14" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="27"/>
+      <c r="B15" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" s="15">
+        <v>44000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A16" s="27"/>
+      <c r="B16" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F13" s="26">
-        <v>45160</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" ht="105" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
-      <c r="B14" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
-      <c r="B15" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="E15" s="28" t="s">
+      <c r="D16" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="F15" s="23">
-        <v>44000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
-      <c r="B16" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D16" s="21" t="s">
+      <c r="E16" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="F16" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="F16" s="29" t="s">
+    </row>
+    <row r="17" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A17" s="27"/>
+      <c r="B17" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="13" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A17" s="12"/>
-      <c r="B17" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D17" s="21" t="s">
+      <c r="E17" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="F17" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="E17" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="F17" s="27" t="s">
+    </row>
+    <row r="18" spans="1:25" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A18" s="27"/>
+      <c r="B18" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="13" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="18" spans="1:25" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
-      <c r="B18" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D18" s="21" t="s">
+      <c r="E18" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="F18" s="15" t="s">
         <v>117</v>
-      </c>
-      <c r="F18" s="23" t="s">
-        <v>118</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
@@ -2125,773 +2124,773 @@
       <c r="Y18" s="4"/>
     </row>
     <row r="19" spans="1:25" ht="45" x14ac:dyDescent="0.2">
-      <c r="A19" s="12"/>
-      <c r="B19" s="21" t="s">
+      <c r="A19" s="27"/>
+      <c r="B19" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" s="21" t="s">
+      <c r="C19" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="F19" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="A20" s="27"/>
+      <c r="B20" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="F19" s="23" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A20" s="12"/>
-      <c r="B20" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="D20" s="24" t="s">
+      <c r="E20" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="F20" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="F20" s="24" t="s">
+    </row>
+    <row r="21" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="28" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="21" spans="1:25" s="33" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="13" t="s">
+      <c r="B21" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" ht="60" x14ac:dyDescent="0.2">
+      <c r="A22" s="29"/>
+      <c r="B22" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="B21" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="F21" s="21" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" ht="60" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D22" s="21" t="s">
+      <c r="E22" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="E22" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="F22" s="22" t="str">
+      <c r="F22" s="14" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
     </row>
     <row r="23" spans="1:25" ht="75" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
-      <c r="B23" s="21" t="s">
+      <c r="A23" s="29"/>
+      <c r="B23" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" ht="60" x14ac:dyDescent="0.2">
+      <c r="A24" s="29"/>
+      <c r="B24" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>196</v>
-      </c>
-      <c r="E23" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="F23" s="21" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" ht="60" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
-      <c r="B24" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="21" t="s">
+      <c r="C24" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E24" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="E24" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="F24" s="22" t="str">
+      <c r="F24" s="14" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
     </row>
     <row r="25" spans="1:25" ht="90" x14ac:dyDescent="0.2">
-      <c r="A25" s="14"/>
-      <c r="B25" s="21" t="s">
+      <c r="A25" s="29"/>
+      <c r="B25" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="A26" s="30"/>
+      <c r="B26" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>195</v>
-      </c>
-      <c r="E25" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="F25" s="21" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A26" s="15"/>
-      <c r="B26" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="D26" s="24" t="s">
+      <c r="C26" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="E26" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="E26" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="F26" s="25" t="str">
+      <c r="F26" s="17" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
     </row>
     <row r="27" spans="1:25" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="B27" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D27" s="21" t="s">
+      <c r="E27" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="F27" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A28" s="31"/>
+      <c r="B28" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="F27" s="21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A28" s="16"/>
-      <c r="B28" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D28" s="21" t="s">
+      <c r="E28" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="F28" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="F28" s="23" t="s">
+    </row>
+    <row r="29" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A29" s="31"/>
+      <c r="B29" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="13" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="29" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A29" s="16"/>
-      <c r="B29" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D29" s="21" t="s">
+      <c r="E29" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F29" s="22">
+        <v>44832</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A30" s="31"/>
+      <c r="B30" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="E29" s="21" t="s">
+      <c r="E30" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30" s="22">
+        <v>44832</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A31" s="31"/>
+      <c r="B31" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F31" s="22">
+        <v>44832</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A32" s="31"/>
+      <c r="B32" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="F32" s="13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A33" s="31"/>
+      <c r="B33" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F29" s="30">
+      <c r="D33" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A34" s="31"/>
+      <c r="B34" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+      <c r="A35" s="31"/>
+      <c r="B35" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A36" s="31"/>
+      <c r="B36" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F36" s="22">
         <v>44832</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A30" s="16"/>
-      <c r="B30" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="E30" s="21" t="s">
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A37" s="31"/>
+      <c r="B37" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="C37" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F30" s="30">
-        <v>44832</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A31" s="16"/>
-      <c r="B31" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D31" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="E31" s="21" t="s">
+      <c r="D37" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A38" s="31"/>
+      <c r="B38" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F31" s="30">
-        <v>44832</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A32" s="16"/>
-      <c r="B32" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D32" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="E32" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="F32" s="21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A33" s="16"/>
-      <c r="B33" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D33" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="E33" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="F33" s="21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A34" s="16"/>
-      <c r="B34" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="C34" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D34" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="E34" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="F34" s="21" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="75" x14ac:dyDescent="0.2">
-      <c r="A35" s="16"/>
-      <c r="B35" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="C35" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D35" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="E35" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="F35" s="21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A36" s="16"/>
-      <c r="B36" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D36" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="E36" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="F36" s="30">
-        <v>44832</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A37" s="16"/>
-      <c r="B37" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="C37" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D37" s="21" t="s">
+      <c r="D38" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="E37" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="F37" s="21" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="60" x14ac:dyDescent="0.2">
-      <c r="A38" s="16"/>
-      <c r="B38" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C38" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D38" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="E38" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="F38" s="21" t="b">
+      <c r="E38" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="F38" s="13" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A39" s="16"/>
-      <c r="B39" s="21" t="s">
+      <c r="A39" s="31"/>
+      <c r="B39" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D39" s="21" t="s">
+      <c r="C39" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F39" s="22">
+        <v>44832</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A40" s="31"/>
+      <c r="B40" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="F40" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="E39" s="21" t="s">
+    </row>
+    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A41" s="31"/>
+      <c r="B41" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F39" s="30">
-        <v>44832</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A40" s="16"/>
-      <c r="B40" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D40" s="21" t="s">
+      <c r="D41" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="E40" s="21" t="s">
+      <c r="E41" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="F41" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="F40" s="21" t="s">
+    </row>
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A42" s="31"/>
+      <c r="B42" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="E42" s="13" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A41" s="16"/>
-      <c r="B41" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C41" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D41" s="21" t="s">
+      <c r="F42" s="19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A43" s="31"/>
+      <c r="B43" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="E41" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="F41" s="21" t="s">
+      <c r="C43" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" s="13" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A42" s="16"/>
-      <c r="B42" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C42" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D42" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="E42" s="21" t="s">
-        <v>158</v>
-      </c>
-      <c r="F42" s="27" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A43" s="16"/>
-      <c r="B43" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="C43" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D43" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="E43" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="F43" s="21" t="b">
+      <c r="E43" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="F43" s="13" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="11" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="17" t="s">
+      <c r="A44" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="E44" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="B44" s="20" t="s">
-        <v>190</v>
-      </c>
-      <c r="C44" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="D44" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="E44" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="F44" s="31" t="str">
+      <c r="F44" s="23" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A45" s="18"/>
-      <c r="B45" s="21" t="s">
+      <c r="A45" s="33"/>
+      <c r="B45" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C45" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D45" s="21" t="s">
+      <c r="C45" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F45" s="22">
+        <v>44937</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A46" s="33"/>
+      <c r="B46" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F46" s="22">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A47" s="33"/>
+      <c r="B47" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="C47" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="E45" s="21" t="s">
+      <c r="D47" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F47" s="22">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A48" s="33"/>
+      <c r="B48" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="C48" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F45" s="30">
-        <v>44937</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A46" s="18"/>
-      <c r="B46" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C46" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D46" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="E46" s="21" t="s">
+      <c r="D48" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25" ht="75" x14ac:dyDescent="0.2">
+      <c r="A49" s="33"/>
+      <c r="B49" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F46" s="30">
-        <v>45454</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A47" s="18"/>
-      <c r="B47" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="C47" s="21" t="s">
-        <v>168</v>
-      </c>
-      <c r="D47" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E47" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="F47" s="30">
-        <v>45454</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A48" s="18"/>
-      <c r="B48" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="C48" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D48" s="21" t="s">
+      <c r="D49" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="E48" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="F48" s="21" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="49" spans="1:25" ht="75" x14ac:dyDescent="0.2">
-      <c r="A49" s="18"/>
-      <c r="B49" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C49" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D49" s="21" t="s">
-        <v>173</v>
-      </c>
-      <c r="E49" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="F49" s="22" t="str">
+      <c r="E49" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="F49" s="14" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
     </row>
     <row r="50" spans="1:25" ht="45" x14ac:dyDescent="0.2">
-      <c r="A50" s="18"/>
-      <c r="B50" s="21" t="s">
+      <c r="A50" s="33"/>
+      <c r="B50" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C50" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D50" s="21" t="s">
+      <c r="C50" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="E50" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F50" s="22">
+        <v>44937</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25" ht="45" x14ac:dyDescent="0.2">
+      <c r="A51" s="33"/>
+      <c r="B51" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F51" s="22">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A52" s="33"/>
+      <c r="B52" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C52" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="D52" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F52" s="22">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A53" s="33"/>
+      <c r="B53" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="C53" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D53" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="E50" s="21" t="s">
+      <c r="E53" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="F53" s="22">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25" ht="75" x14ac:dyDescent="0.2">
+      <c r="A54" s="33"/>
+      <c r="B54" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C54" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F50" s="30">
-        <v>44937</v>
-      </c>
-    </row>
-    <row r="51" spans="1:25" ht="45" x14ac:dyDescent="0.2">
-      <c r="A51" s="18"/>
-      <c r="B51" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C51" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D51" s="21" t="s">
+      <c r="D54" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="E51" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="F51" s="30">
-        <v>45454</v>
-      </c>
-    </row>
-    <row r="52" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A52" s="18"/>
-      <c r="B52" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="C52" s="32" t="s">
-        <v>168</v>
-      </c>
-      <c r="D52" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="E52" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="F52" s="30">
-        <v>45454</v>
-      </c>
-    </row>
-    <row r="53" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A53" s="18"/>
-      <c r="B53" s="21" t="s">
-        <v>192</v>
-      </c>
-      <c r="C53" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="D53" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="E53" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="F53" s="30">
-        <v>45454</v>
-      </c>
-    </row>
-    <row r="54" spans="1:25" ht="75" x14ac:dyDescent="0.2">
-      <c r="A54" s="18"/>
-      <c r="B54" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C54" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D54" s="21" t="s">
-        <v>178</v>
-      </c>
-      <c r="E54" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="F54" s="22" t="str">
+      <c r="E54" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="F54" s="14" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
     </row>
     <row r="55" spans="1:25" ht="45" x14ac:dyDescent="0.2">
-      <c r="A55" s="18"/>
-      <c r="B55" s="21" t="s">
+      <c r="A55" s="33"/>
+      <c r="B55" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C55" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D55" s="21" t="s">
+      <c r="C55" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D55" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="E55" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F55" s="22">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="56" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A56" s="33"/>
+      <c r="B56" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D56" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="E56" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F56" s="22">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="57" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A57" s="33"/>
+      <c r="B57" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="D57" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="E57" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F57" s="22">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="58" spans="1:25" ht="30" x14ac:dyDescent="0.2">
+      <c r="A58" s="33"/>
+      <c r="B58" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D58" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="E55" s="21" t="s">
+      <c r="E58" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F58" s="13" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25" ht="75" x14ac:dyDescent="0.2">
+      <c r="A59" s="33"/>
+      <c r="B59" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C59" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F55" s="30">
-        <v>45454</v>
-      </c>
-    </row>
-    <row r="56" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A56" s="18"/>
-      <c r="B56" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C56" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D56" s="21" t="s">
-        <v>180</v>
-      </c>
-      <c r="E56" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="F56" s="30">
-        <v>45454</v>
-      </c>
-    </row>
-    <row r="57" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A57" s="18"/>
-      <c r="B57" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C57" s="21" t="s">
-        <v>168</v>
-      </c>
-      <c r="D57" s="21" t="s">
+      <c r="D59" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="E57" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="F57" s="30">
-        <v>45454</v>
-      </c>
-    </row>
-    <row r="58" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A58" s="18"/>
-      <c r="B58" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="C58" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D58" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="E58" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="F58" s="21" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="59" spans="1:25" ht="75" x14ac:dyDescent="0.2">
-      <c r="A59" s="18"/>
-      <c r="B59" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C59" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D59" s="21" t="s">
-        <v>184</v>
-      </c>
-      <c r="E59" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="F59" s="22" t="str">
+      <c r="E59" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="F59" s="14" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
     </row>
     <row r="60" spans="1:25" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A60" s="18"/>
-      <c r="B60" s="21" t="s">
+      <c r="A60" s="33"/>
+      <c r="B60" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C60" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D60" s="21" t="s">
-        <v>185</v>
-      </c>
-      <c r="E60" s="21" t="s">
+      <c r="C60" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F60" s="30">
+      <c r="D60" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="E60" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F60" s="22">
         <v>45454</v>
       </c>
       <c r="G60" s="4"/>
@@ -2915,57 +2914,57 @@
       <c r="Y60" s="4"/>
     </row>
     <row r="61" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A61" s="18"/>
-      <c r="B61" s="21" t="s">
+      <c r="A61" s="33"/>
+      <c r="B61" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C61" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D61" s="21" t="s">
-        <v>186</v>
-      </c>
-      <c r="E61" s="21" t="s">
+      <c r="C61" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F61" s="30">
+      <c r="D61" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="E61" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F61" s="22">
         <v>45454</v>
       </c>
     </row>
     <row r="62" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A62" s="18"/>
-      <c r="B62" s="21" t="s">
+      <c r="A62" s="33"/>
+      <c r="B62" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C62" s="21" t="s">
-        <v>168</v>
-      </c>
-      <c r="D62" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="E62" s="21" t="s">
+      <c r="C62" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="D62" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="E62" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F62" s="22">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="63" spans="1:25" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A63" s="34"/>
+      <c r="B63" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C63" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="F62" s="30">
-        <v>45454</v>
-      </c>
-    </row>
-    <row r="63" spans="1:25" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A63" s="19"/>
-      <c r="B63" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C63" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="D63" s="24" t="s">
-        <v>188</v>
-      </c>
-      <c r="E63" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="F63" s="24" t="s">
-        <v>183</v>
+      <c r="D63" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="E63" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="F63" s="16" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix: mise à jour excel (siret employeur et message sur l'année en cours)
</commit_message>
<xml_diff>
--- a/ui/public/modele-import.xlsx
+++ b/ui/public/modele-import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raph/dev/flux-retour-cfas/ui/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25C40EE-7344-ED4A-8271-3EE29CB38492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7789EE45-3267-5946-AA45-F679FBF6EB58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="500" windowWidth="27660" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Modèle" sheetId="1" r:id="rId1"/>
     <sheet name="Description des données" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -180,9 +180,6 @@
     <t>cause_rupture_contrat_4</t>
   </si>
   <si>
-    <t>siret_employeur</t>
-  </si>
-  <si>
     <t>siret_employeur_2</t>
   </si>
   <si>
@@ -436,9 +433,6 @@
     <t>AAAA-AAAA</t>
   </si>
   <si>
-    <t>année de formation concernée</t>
-  </si>
-  <si>
     <t>Énumération : 1, 2, 3, 4, 5</t>
   </si>
   <si>
@@ -621,10 +615,6 @@
     <t>code_postal_apprenant</t>
   </si>
   <si>
-    <t xml:space="preserve">siret_employeur
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">cause_rupture_contrat
 </t>
   </si>
@@ -653,6 +643,16 @@
   </si>
   <si>
     <t>duree_theorique_formation_mois *</t>
+  </si>
+  <si>
+    <t>siret_employeur *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">siret_employeur *
+</t>
+  </si>
+  <si>
+    <t>Année de formation concernée. Se référer à la notice SIFA pour plus de précisions, disponible dans l’onglet "Mon enquête SIFA".</t>
   </si>
 </sst>
 </file>
@@ -1365,7 +1365,7 @@
     <col min="42" max="42" width="26" style="1" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="14.5" style="1" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.5" style="1" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -1442,22 +1442,22 @@
         <v>26</v>
       </c>
       <c r="T1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="U1" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="W1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>59</v>
-      </c>
-      <c r="Y1" s="7" t="s">
-        <v>60</v>
       </c>
       <c r="Z1" s="9" t="s">
         <v>4</v>
@@ -1472,16 +1472,16 @@
         <v>13</v>
       </c>
       <c r="AD1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="AE1" s="9" t="s">
+      <c r="AF1" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="AF1" s="9" t="s">
-        <v>54</v>
-      </c>
       <c r="AG1" s="9" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="AH1" s="9" t="s">
         <v>10</v>
@@ -1499,7 +1499,7 @@
         <v>30</v>
       </c>
       <c r="AM1" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AN1" s="9" t="s">
         <v>31</v>
@@ -1517,7 +1517,7 @@
         <v>15</v>
       </c>
       <c r="AS1" s="10" t="s">
-        <v>47</v>
+        <v>194</v>
       </c>
       <c r="AT1" s="10" t="s">
         <v>16</v>
@@ -1532,7 +1532,7 @@
         <v>36</v>
       </c>
       <c r="AX1" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AY1" s="10" t="s">
         <v>37</v>
@@ -1547,7 +1547,7 @@
         <v>40</v>
       </c>
       <c r="BC1" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BD1" s="10" t="s">
         <v>41</v>
@@ -1562,7 +1562,7 @@
         <v>44</v>
       </c>
       <c r="BH1" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="BI1" s="10" t="s">
         <v>45</v>
@@ -1573,10 +1573,10 @@
     </row>
     <row r="2" spans="1:62" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
@@ -1588,29 +1588,29 @@
         <v>36827</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G2" s="2">
         <v>44400</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J2" s="2">
         <v>44000</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L2" s="2" t="str">
         <f>"1234567890123"</f>
         <v>1234567890123</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N2" s="2" t="b">
         <f>TRUE()</f>
@@ -1620,46 +1620,46 @@
         <v>40479</v>
       </c>
       <c r="P2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="S2" s="2">
         <v>4101</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U2" s="2" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="W2" s="2" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Y2" s="2" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AA2" s="2">
         <v>1</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AC2" s="2" t="str">
         <f>"50022141"</f>
@@ -1678,7 +1678,7 @@
         <v>24</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AI2" s="2" t="b">
         <f>TRUE()</f>
@@ -1708,7 +1708,7 @@
         <v>45087</v>
       </c>
       <c r="AU2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AV2" s="3">
         <v>44937</v>
@@ -1742,8 +1742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y978"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1760,19 +1760,19 @@
     <row r="1" spans="1:25" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="25"/>
       <c r="B1" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="F1" s="26" t="s">
         <v>77</v>
-      </c>
-      <c r="F1" s="26" t="s">
-        <v>78</v>
       </c>
       <c r="G1" s="25"/>
       <c r="H1" s="25"/>
@@ -1796,22 +1796,22 @@
     </row>
     <row r="2" spans="1:25" ht="60" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="E2" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>82</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="60" x14ac:dyDescent="0.2">
@@ -1820,16 +1820,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="30" x14ac:dyDescent="0.2">
@@ -1838,13 +1838,13 @@
         <v>2</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D4" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>85</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>86</v>
       </c>
       <c r="F4" s="18">
         <v>35819</v>
@@ -1856,13 +1856,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="E5" s="13" t="s">
         <v>88</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>89</v>
       </c>
       <c r="F5" s="15">
         <v>44400</v>
@@ -1874,13 +1874,13 @@
         <v>6</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F6" s="18">
         <v>35819</v>
@@ -1892,13 +1892,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D7" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>91</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>92</v>
       </c>
       <c r="F7" s="13">
         <v>2</v>
@@ -1910,16 +1910,16 @@
         <v>8</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D8" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>94</v>
-      </c>
       <c r="F8" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="105" x14ac:dyDescent="0.2">
@@ -1928,16 +1928,16 @@
         <v>9</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D9" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="F9" s="13" t="s">
         <v>96</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="45" x14ac:dyDescent="0.2">
@@ -1946,31 +1946,31 @@
         <v>7</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D10" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="E10" s="13" t="s">
-        <v>99</v>
-      </c>
       <c r="F10" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="60" x14ac:dyDescent="0.2">
       <c r="A11" s="27"/>
       <c r="B11" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" s="13" t="s">
+      <c r="E11" s="13" t="s">
         <v>101</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>102</v>
       </c>
       <c r="F11" s="13" t="str">
         <f>"1234567890123"</f>
@@ -1983,13 +1983,13 @@
         <v>21</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D12" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>103</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>104</v>
       </c>
       <c r="F12" s="13" t="b">
         <f>TRUE()</f>
@@ -2002,13 +2002,13 @@
         <v>22</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F13" s="18">
         <v>45160</v>
@@ -2020,31 +2020,31 @@
         <v>18</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D14" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="E14" s="13" t="s">
-        <v>107</v>
-      </c>
       <c r="F14" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="27"/>
       <c r="B15" s="13" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D15" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="20" t="s">
         <v>108</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>109</v>
       </c>
       <c r="F15" s="15">
         <v>44000</v>
@@ -2056,16 +2056,16 @@
         <v>23</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D16" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="E16" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="F16" s="21" t="s">
         <v>111</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="30" x14ac:dyDescent="0.2">
@@ -2074,16 +2074,16 @@
         <v>24</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D17" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="F17" s="19" t="s">
         <v>113</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:25" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -2092,16 +2092,16 @@
         <v>20</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D18" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="F18" s="15" t="s">
         <v>116</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>117</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
@@ -2129,16 +2129,16 @@
         <v>25</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D19" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="E19" s="15" t="s">
-        <v>119</v>
-      </c>
       <c r="F19" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:25" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
@@ -2147,51 +2147,51 @@
         <v>26</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D20" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="F20" s="16" t="s">
         <v>121</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:25" ht="60" x14ac:dyDescent="0.2">
       <c r="A22" s="29"/>
       <c r="B22" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D22" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E22" s="13" t="s">
         <v>124</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>125</v>
       </c>
       <c r="F22" s="14" t="str">
         <f>"12345678901235"</f>
@@ -2201,34 +2201,34 @@
     <row r="23" spans="1:25" ht="75" x14ac:dyDescent="0.2">
       <c r="A23" s="29"/>
       <c r="B23" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:25" ht="60" x14ac:dyDescent="0.2">
       <c r="A24" s="29"/>
       <c r="B24" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D24" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E24" s="13" t="s">
         <v>124</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>125</v>
       </c>
       <c r="F24" s="14" t="str">
         <f>"12345678901235"</f>
@@ -2238,34 +2238,34 @@
     <row r="25" spans="1:25" ht="90" x14ac:dyDescent="0.2">
       <c r="A25" s="29"/>
       <c r="B25" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:25" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A26" s="30"/>
       <c r="B26" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D26" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="E26" s="16" t="s">
         <v>124</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>125</v>
       </c>
       <c r="F26" s="17" t="str">
         <f>"12345678901235"</f>
@@ -2274,22 +2274,22 @@
     </row>
     <row r="27" spans="1:25" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B27" s="13" t="s">
         <v>4</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D27" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="E27" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="E27" s="13" t="s">
-        <v>128</v>
-      </c>
       <c r="F27" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:25" ht="30" x14ac:dyDescent="0.2">
@@ -2298,31 +2298,31 @@
         <v>11</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D28" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="F28" s="15" t="s">
         <v>129</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="31"/>
       <c r="B29" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F29" s="22">
         <v>44832</v>
@@ -2331,16 +2331,16 @@
     <row r="30" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" s="31"/>
       <c r="B30" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F30" s="22">
         <v>44832</v>
@@ -2349,16 +2349,16 @@
     <row r="31" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" s="31"/>
       <c r="B31" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F31" s="22">
         <v>44832</v>
@@ -2367,16 +2367,16 @@
     <row r="32" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" s="31"/>
       <c r="B32" s="13" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F32" s="13">
         <v>12</v>
@@ -2388,52 +2388,52 @@
         <v>10</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A34" s="31"/>
       <c r="B34" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="F34" s="13" t="s">
         <v>137</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="F34" s="13" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="75" x14ac:dyDescent="0.2">
       <c r="A35" s="31"/>
       <c r="B35" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="E35" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="C35" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D35" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>142</v>
-      </c>
       <c r="F35" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -2442,13 +2442,13 @@
         <v>29</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E36" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F36" s="22">
         <v>44832</v>
@@ -2457,19 +2457,19 @@
     <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A37" s="31"/>
       <c r="B37" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="E37" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="C37" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D37" s="13" t="s">
+      <c r="F37" s="13" t="s">
         <v>145</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F37" s="13" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="60" x14ac:dyDescent="0.2">
@@ -2478,13 +2478,13 @@
         <v>27</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F38" s="13" t="b">
         <f>TRUE()</f>
@@ -2497,13 +2497,13 @@
         <v>28</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F39" s="22">
         <v>44832</v>
@@ -2515,16 +2515,16 @@
         <v>31</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D40" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="F40" s="13" t="s">
         <v>150</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="F40" s="13" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -2533,16 +2533,16 @@
         <v>32</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -2551,31 +2551,31 @@
         <v>33</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F42" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" s="31"/>
       <c r="B43" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F43" s="13" t="b">
         <f>TRUE()</f>
@@ -2584,19 +2584,19 @@
     </row>
     <row r="44" spans="1:6" s="11" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D44" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="B44" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="C44" s="12" t="s">
+      <c r="E44" s="12" t="s">
         <v>159</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>161</v>
       </c>
       <c r="F44" s="23" t="str">
         <f>"12345678901235"</f>
@@ -2609,13 +2609,13 @@
         <v>14</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F45" s="22">
         <v>44937</v>
@@ -2627,13 +2627,13 @@
         <v>15</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F46" s="22">
         <v>45454</v>
@@ -2642,16 +2642,16 @@
     <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A47" s="33"/>
       <c r="B47" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D47" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="C47" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>166</v>
-      </c>
       <c r="E47" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F47" s="22">
         <v>45454</v>
@@ -2660,34 +2660,34 @@
     <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" s="33"/>
       <c r="B48" s="13" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D48" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="F48" s="13" t="s">
         <v>167</v>
-      </c>
-      <c r="E48" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="F48" s="13" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="49" spans="1:25" ht="75" x14ac:dyDescent="0.2">
       <c r="A49" s="33"/>
       <c r="B49" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F49" s="14" t="str">
         <f>"12345678901235"</f>
@@ -2700,13 +2700,13 @@
         <v>35</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F50" s="22">
         <v>44937</v>
@@ -2718,13 +2718,13 @@
         <v>36</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F51" s="22">
         <v>45454</v>
@@ -2736,13 +2736,13 @@
         <v>37</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F52" s="22">
         <v>45454</v>
@@ -2751,16 +2751,16 @@
     <row r="53" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A53" s="33"/>
       <c r="B53" s="13" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C53" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D53" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F53" s="22">
         <v>45454</v>
@@ -2769,16 +2769,16 @@
     <row r="54" spans="1:25" ht="75" x14ac:dyDescent="0.2">
       <c r="A54" s="33"/>
       <c r="B54" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D54" s="13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E54" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F54" s="14" t="str">
         <f>"12345678901235"</f>
@@ -2791,13 +2791,13 @@
         <v>39</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D55" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E55" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F55" s="22">
         <v>45454</v>
@@ -2809,13 +2809,13 @@
         <v>40</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D56" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E56" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F56" s="22">
         <v>45454</v>
@@ -2827,13 +2827,13 @@
         <v>41</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D57" s="13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E57" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F57" s="22">
         <v>45454</v>
@@ -2842,34 +2842,34 @@
     <row r="58" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A58" s="33"/>
       <c r="B58" s="13" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E58" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F58" s="13" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="59" spans="1:25" ht="75" x14ac:dyDescent="0.2">
       <c r="A59" s="33"/>
       <c r="B59" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E59" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F59" s="14" t="str">
         <f>"12345678901235"</f>
@@ -2882,13 +2882,13 @@
         <v>43</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E60" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F60" s="22">
         <v>45454</v>
@@ -2919,13 +2919,13 @@
         <v>44</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E61" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F61" s="22">
         <v>45454</v>
@@ -2937,13 +2937,13 @@
         <v>45</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D62" s="13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E62" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F62" s="22">
         <v>45454</v>
@@ -2955,16 +2955,16 @@
         <v>46</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D63" s="16" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E63" s="16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F63" s="16" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix: mise à jour excel (siret employeur et message sur l'année en cours) (#3409)
</commit_message>
<xml_diff>
--- a/ui/public/modele-import.xlsx
+++ b/ui/public/modele-import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raph/dev/flux-retour-cfas/ui/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25C40EE-7344-ED4A-8271-3EE29CB38492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7789EE45-3267-5946-AA45-F679FBF6EB58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="500" windowWidth="27660" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Modèle" sheetId="1" r:id="rId1"/>
     <sheet name="Description des données" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -180,9 +180,6 @@
     <t>cause_rupture_contrat_4</t>
   </si>
   <si>
-    <t>siret_employeur</t>
-  </si>
-  <si>
     <t>siret_employeur_2</t>
   </si>
   <si>
@@ -436,9 +433,6 @@
     <t>AAAA-AAAA</t>
   </si>
   <si>
-    <t>année de formation concernée</t>
-  </si>
-  <si>
     <t>Énumération : 1, 2, 3, 4, 5</t>
   </si>
   <si>
@@ -621,10 +615,6 @@
     <t>code_postal_apprenant</t>
   </si>
   <si>
-    <t xml:space="preserve">siret_employeur
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">cause_rupture_contrat
 </t>
   </si>
@@ -653,6 +643,16 @@
   </si>
   <si>
     <t>duree_theorique_formation_mois *</t>
+  </si>
+  <si>
+    <t>siret_employeur *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">siret_employeur *
+</t>
+  </si>
+  <si>
+    <t>Année de formation concernée. Se référer à la notice SIFA pour plus de précisions, disponible dans l’onglet "Mon enquête SIFA".</t>
   </si>
 </sst>
 </file>
@@ -1365,7 +1365,7 @@
     <col min="42" max="42" width="26" style="1" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="14.5" style="1" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.5" style="1" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -1442,22 +1442,22 @@
         <v>26</v>
       </c>
       <c r="T1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="U1" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="W1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>59</v>
-      </c>
-      <c r="Y1" s="7" t="s">
-        <v>60</v>
       </c>
       <c r="Z1" s="9" t="s">
         <v>4</v>
@@ -1472,16 +1472,16 @@
         <v>13</v>
       </c>
       <c r="AD1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="AE1" s="9" t="s">
+      <c r="AF1" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="AF1" s="9" t="s">
-        <v>54</v>
-      </c>
       <c r="AG1" s="9" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="AH1" s="9" t="s">
         <v>10</v>
@@ -1499,7 +1499,7 @@
         <v>30</v>
       </c>
       <c r="AM1" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AN1" s="9" t="s">
         <v>31</v>
@@ -1517,7 +1517,7 @@
         <v>15</v>
       </c>
       <c r="AS1" s="10" t="s">
-        <v>47</v>
+        <v>194</v>
       </c>
       <c r="AT1" s="10" t="s">
         <v>16</v>
@@ -1532,7 +1532,7 @@
         <v>36</v>
       </c>
       <c r="AX1" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AY1" s="10" t="s">
         <v>37</v>
@@ -1547,7 +1547,7 @@
         <v>40</v>
       </c>
       <c r="BC1" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BD1" s="10" t="s">
         <v>41</v>
@@ -1562,7 +1562,7 @@
         <v>44</v>
       </c>
       <c r="BH1" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="BI1" s="10" t="s">
         <v>45</v>
@@ -1573,10 +1573,10 @@
     </row>
     <row r="2" spans="1:62" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
@@ -1588,29 +1588,29 @@
         <v>36827</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G2" s="2">
         <v>44400</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J2" s="2">
         <v>44000</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L2" s="2" t="str">
         <f>"1234567890123"</f>
         <v>1234567890123</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N2" s="2" t="b">
         <f>TRUE()</f>
@@ -1620,46 +1620,46 @@
         <v>40479</v>
       </c>
       <c r="P2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="S2" s="2">
         <v>4101</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U2" s="2" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="W2" s="2" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Y2" s="2" t="str">
         <f>"12345678901235"</f>
         <v>12345678901235</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AA2" s="2">
         <v>1</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AC2" s="2" t="str">
         <f>"50022141"</f>
@@ -1678,7 +1678,7 @@
         <v>24</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AI2" s="2" t="b">
         <f>TRUE()</f>
@@ -1708,7 +1708,7 @@
         <v>45087</v>
       </c>
       <c r="AU2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AV2" s="3">
         <v>44937</v>
@@ -1742,8 +1742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y978"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1760,19 +1760,19 @@
     <row r="1" spans="1:25" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="25"/>
       <c r="B1" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="F1" s="26" t="s">
         <v>77</v>
-      </c>
-      <c r="F1" s="26" t="s">
-        <v>78</v>
       </c>
       <c r="G1" s="25"/>
       <c r="H1" s="25"/>
@@ -1796,22 +1796,22 @@
     </row>
     <row r="2" spans="1:25" ht="60" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="E2" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>82</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="60" x14ac:dyDescent="0.2">
@@ -1820,16 +1820,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="30" x14ac:dyDescent="0.2">
@@ -1838,13 +1838,13 @@
         <v>2</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D4" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>85</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>86</v>
       </c>
       <c r="F4" s="18">
         <v>35819</v>
@@ -1856,13 +1856,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="E5" s="13" t="s">
         <v>88</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>89</v>
       </c>
       <c r="F5" s="15">
         <v>44400</v>
@@ -1874,13 +1874,13 @@
         <v>6</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F6" s="18">
         <v>35819</v>
@@ -1892,13 +1892,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D7" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>91</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>92</v>
       </c>
       <c r="F7" s="13">
         <v>2</v>
@@ -1910,16 +1910,16 @@
         <v>8</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D8" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>94</v>
-      </c>
       <c r="F8" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="105" x14ac:dyDescent="0.2">
@@ -1928,16 +1928,16 @@
         <v>9</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D9" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="F9" s="13" t="s">
         <v>96</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="45" x14ac:dyDescent="0.2">
@@ -1946,31 +1946,31 @@
         <v>7</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D10" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="E10" s="13" t="s">
-        <v>99</v>
-      </c>
       <c r="F10" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="60" x14ac:dyDescent="0.2">
       <c r="A11" s="27"/>
       <c r="B11" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" s="13" t="s">
+      <c r="E11" s="13" t="s">
         <v>101</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>102</v>
       </c>
       <c r="F11" s="13" t="str">
         <f>"1234567890123"</f>
@@ -1983,13 +1983,13 @@
         <v>21</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D12" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>103</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>104</v>
       </c>
       <c r="F12" s="13" t="b">
         <f>TRUE()</f>
@@ -2002,13 +2002,13 @@
         <v>22</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F13" s="18">
         <v>45160</v>
@@ -2020,31 +2020,31 @@
         <v>18</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D14" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="E14" s="13" t="s">
-        <v>107</v>
-      </c>
       <c r="F14" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="27"/>
       <c r="B15" s="13" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D15" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="20" t="s">
         <v>108</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>109</v>
       </c>
       <c r="F15" s="15">
         <v>44000</v>
@@ -2056,16 +2056,16 @@
         <v>23</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D16" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="E16" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="F16" s="21" t="s">
         <v>111</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="30" x14ac:dyDescent="0.2">
@@ -2074,16 +2074,16 @@
         <v>24</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D17" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="F17" s="19" t="s">
         <v>113</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:25" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -2092,16 +2092,16 @@
         <v>20</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D18" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="F18" s="15" t="s">
         <v>116</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>117</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
@@ -2129,16 +2129,16 @@
         <v>25</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D19" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="E19" s="15" t="s">
-        <v>119</v>
-      </c>
       <c r="F19" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:25" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
@@ -2147,51 +2147,51 @@
         <v>26</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D20" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="F20" s="16" t="s">
         <v>121</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:25" ht="60" x14ac:dyDescent="0.2">
       <c r="A22" s="29"/>
       <c r="B22" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D22" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E22" s="13" t="s">
         <v>124</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>125</v>
       </c>
       <c r="F22" s="14" t="str">
         <f>"12345678901235"</f>
@@ -2201,34 +2201,34 @@
     <row r="23" spans="1:25" ht="75" x14ac:dyDescent="0.2">
       <c r="A23" s="29"/>
       <c r="B23" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:25" ht="60" x14ac:dyDescent="0.2">
       <c r="A24" s="29"/>
       <c r="B24" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D24" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E24" s="13" t="s">
         <v>124</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>125</v>
       </c>
       <c r="F24" s="14" t="str">
         <f>"12345678901235"</f>
@@ -2238,34 +2238,34 @@
     <row r="25" spans="1:25" ht="90" x14ac:dyDescent="0.2">
       <c r="A25" s="29"/>
       <c r="B25" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:25" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A26" s="30"/>
       <c r="B26" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D26" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="E26" s="16" t="s">
         <v>124</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>125</v>
       </c>
       <c r="F26" s="17" t="str">
         <f>"12345678901235"</f>
@@ -2274,22 +2274,22 @@
     </row>
     <row r="27" spans="1:25" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B27" s="13" t="s">
         <v>4</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D27" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="E27" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="E27" s="13" t="s">
-        <v>128</v>
-      </c>
       <c r="F27" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:25" ht="30" x14ac:dyDescent="0.2">
@@ -2298,31 +2298,31 @@
         <v>11</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D28" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="F28" s="15" t="s">
         <v>129</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="31"/>
       <c r="B29" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F29" s="22">
         <v>44832</v>
@@ -2331,16 +2331,16 @@
     <row r="30" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" s="31"/>
       <c r="B30" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F30" s="22">
         <v>44832</v>
@@ -2349,16 +2349,16 @@
     <row r="31" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" s="31"/>
       <c r="B31" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F31" s="22">
         <v>44832</v>
@@ -2367,16 +2367,16 @@
     <row r="32" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" s="31"/>
       <c r="B32" s="13" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F32" s="13">
         <v>12</v>
@@ -2388,52 +2388,52 @@
         <v>10</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A34" s="31"/>
       <c r="B34" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="F34" s="13" t="s">
         <v>137</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="F34" s="13" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="75" x14ac:dyDescent="0.2">
       <c r="A35" s="31"/>
       <c r="B35" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="E35" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="C35" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D35" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>142</v>
-      </c>
       <c r="F35" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -2442,13 +2442,13 @@
         <v>29</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E36" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F36" s="22">
         <v>44832</v>
@@ -2457,19 +2457,19 @@
     <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A37" s="31"/>
       <c r="B37" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="E37" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="C37" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D37" s="13" t="s">
+      <c r="F37" s="13" t="s">
         <v>145</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F37" s="13" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="60" x14ac:dyDescent="0.2">
@@ -2478,13 +2478,13 @@
         <v>27</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F38" s="13" t="b">
         <f>TRUE()</f>
@@ -2497,13 +2497,13 @@
         <v>28</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F39" s="22">
         <v>44832</v>
@@ -2515,16 +2515,16 @@
         <v>31</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D40" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="F40" s="13" t="s">
         <v>150</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="F40" s="13" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -2533,16 +2533,16 @@
         <v>32</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -2551,31 +2551,31 @@
         <v>33</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F42" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" s="31"/>
       <c r="B43" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F43" s="13" t="b">
         <f>TRUE()</f>
@@ -2584,19 +2584,19 @@
     </row>
     <row r="44" spans="1:6" s="11" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D44" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="B44" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="C44" s="12" t="s">
+      <c r="E44" s="12" t="s">
         <v>159</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>161</v>
       </c>
       <c r="F44" s="23" t="str">
         <f>"12345678901235"</f>
@@ -2609,13 +2609,13 @@
         <v>14</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F45" s="22">
         <v>44937</v>
@@ -2627,13 +2627,13 @@
         <v>15</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F46" s="22">
         <v>45454</v>
@@ -2642,16 +2642,16 @@
     <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A47" s="33"/>
       <c r="B47" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D47" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="C47" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>166</v>
-      </c>
       <c r="E47" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F47" s="22">
         <v>45454</v>
@@ -2660,34 +2660,34 @@
     <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" s="33"/>
       <c r="B48" s="13" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D48" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="F48" s="13" t="s">
         <v>167</v>
-      </c>
-      <c r="E48" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="F48" s="13" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="49" spans="1:25" ht="75" x14ac:dyDescent="0.2">
       <c r="A49" s="33"/>
       <c r="B49" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F49" s="14" t="str">
         <f>"12345678901235"</f>
@@ -2700,13 +2700,13 @@
         <v>35</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F50" s="22">
         <v>44937</v>
@@ -2718,13 +2718,13 @@
         <v>36</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F51" s="22">
         <v>45454</v>
@@ -2736,13 +2736,13 @@
         <v>37</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F52" s="22">
         <v>45454</v>
@@ -2751,16 +2751,16 @@
     <row r="53" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A53" s="33"/>
       <c r="B53" s="13" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C53" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D53" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F53" s="22">
         <v>45454</v>
@@ -2769,16 +2769,16 @@
     <row r="54" spans="1:25" ht="75" x14ac:dyDescent="0.2">
       <c r="A54" s="33"/>
       <c r="B54" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D54" s="13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E54" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F54" s="14" t="str">
         <f>"12345678901235"</f>
@@ -2791,13 +2791,13 @@
         <v>39</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D55" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E55" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F55" s="22">
         <v>45454</v>
@@ -2809,13 +2809,13 @@
         <v>40</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D56" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E56" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F56" s="22">
         <v>45454</v>
@@ -2827,13 +2827,13 @@
         <v>41</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D57" s="13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E57" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F57" s="22">
         <v>45454</v>
@@ -2842,34 +2842,34 @@
     <row r="58" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A58" s="33"/>
       <c r="B58" s="13" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E58" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F58" s="13" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="59" spans="1:25" ht="75" x14ac:dyDescent="0.2">
       <c r="A59" s="33"/>
       <c r="B59" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E59" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F59" s="14" t="str">
         <f>"12345678901235"</f>
@@ -2882,13 +2882,13 @@
         <v>43</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E60" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F60" s="22">
         <v>45454</v>
@@ -2919,13 +2919,13 @@
         <v>44</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E61" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F61" s="22">
         <v>45454</v>
@@ -2937,13 +2937,13 @@
         <v>45</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D62" s="13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E62" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F62" s="22">
         <v>45454</v>
@@ -2955,16 +2955,16 @@
         <v>46</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D63" s="16" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E63" s="16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F63" s="16" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.2">

</xml_diff>